<commit_message>
Started CAD and basic frames
</commit_message>
<xml_diff>
--- a/BOM/BillOfMaterials.xlsx
+++ b/BOM/BillOfMaterials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reger\Documents\Project\Schistoscope\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reger\Documents\Project\Flex Delft Work\Open Hardware\Schistoscope\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029042FC-662C-4586-B1FC-EA001670AE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279B9ED5-FF2F-4982-AEE1-EEA6DC6E0175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{E17B2124-711C-4341-A725-6D6BA9A2AA94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="251">
   <si>
     <t>Name</t>
   </si>
@@ -718,6 +718,75 @@
   </si>
   <si>
     <t>https://nl.aliexpress.com/item/32817786051.html?spm=a2g0o.order_list.order_list_main.424.3cbe79d2ZJ7jjH&amp;gatewayAdapt=glo2nld</t>
+  </si>
+  <si>
+    <t>Bought 250</t>
+  </si>
+  <si>
+    <t>Set of 50</t>
+  </si>
+  <si>
+    <t>Different</t>
+  </si>
+  <si>
+    <t>10 set</t>
+  </si>
+  <si>
+    <t>12 Set Size unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium </t>
+  </si>
+  <si>
+    <t>Bought Set</t>
+  </si>
+  <si>
+    <t>Bought set</t>
+  </si>
+  <si>
+    <t>OD4 L4</t>
+  </si>
+  <si>
+    <t>OD5 L5</t>
+  </si>
+  <si>
+    <t>Multiple color 5m</t>
+  </si>
+  <si>
+    <t>Pins?</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>Size? Buying 300mm</t>
+  </si>
+  <si>
+    <t>3W and 1W</t>
+  </si>
+  <si>
+    <t>DRV and TMC</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Check Pi</t>
+  </si>
+  <si>
+    <t>Check wrong link</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005004082657333.html?spm=a2g0o.productlist.main.3.4c7272f1OFxzgC&amp;algo_pvid=726133d7-3067-4dd9-be70-fd90f83b1e7c&amp;algo_exp_id=726133d7-3067-4dd9-be70-fd90f83b1e7c-1&amp;pdp_npi=4%40dis%21EUR%215.92%215.92%21%21%216.16%21%21%40210318b816956465321157888e3686%2112000029757433927%21sea%21NL%21822878130%21AC&amp;curPageLogUid=9AYYNr9hrC1j</t>
+  </si>
+  <si>
+    <t>Wrong line</t>
+  </si>
+  <si>
+    <t>Bought from farnell</t>
+  </si>
+  <si>
+    <t>Farnelll</t>
   </si>
 </sst>
 </file>
@@ -728,7 +797,7 @@
     <numFmt numFmtId="164" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,8 +841,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,7 +931,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,7 +986,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,9 +1035,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -929,27 +1045,6 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -963,15 +1058,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1290,2882 +1433,3026 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6BBD35-C26C-4525-ACA8-90589C56027B}">
-  <dimension ref="A1:K135"/>
+  <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="23.1328125" customWidth="1"/>
-    <col min="3" max="3" width="28.19921875" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.1328125" customWidth="1"/>
-    <col min="7" max="7" width="22.1328125" customWidth="1"/>
-    <col min="9" max="9" width="12.46484375" customWidth="1"/>
-    <col min="11" max="11" width="91.1328125" customWidth="1"/>
-    <col min="12" max="12" width="8.53125" customWidth="1"/>
+    <col min="3" max="3" width="23.1328125" customWidth="1"/>
+    <col min="4" max="4" width="28.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" customWidth="1"/>
+    <col min="8" max="8" width="22.1328125" customWidth="1"/>
+    <col min="10" max="10" width="12.46484375" customWidth="1"/>
+    <col min="12" max="12" width="91.1328125" customWidth="1"/>
+    <col min="13" max="13" width="8.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="14">
-        <f>SUM(G:G)</f>
+      <c r="K1" s="14">
+        <f>SUM(H:H)</f>
         <v>799.2317700000001</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+    <row r="3" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="16">
+      <c r="E3" s="41">
         <v>2</v>
       </c>
-      <c r="E3" s="26">
+      <c r="F3" s="43">
         <v>24.59</v>
       </c>
-      <c r="F3" s="27">
+      <c r="G3" s="44">
         <v>24.2</v>
       </c>
-      <c r="G3" s="15">
-        <f>D3*E3+F3</f>
+      <c r="H3" s="45">
+        <f>E3*F3+G3</f>
         <v>73.38</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="46" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
+    <row r="4" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="41">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="D4" s="16">
+      <c r="E4" s="41">
         <v>1</v>
       </c>
-      <c r="E4" s="14">
+      <c r="F4" s="44">
         <v>25.1</v>
       </c>
-      <c r="F4" s="27">
+      <c r="G4" s="44">
         <v>5.61</v>
       </c>
-      <c r="G4" s="15">
-        <f t="shared" ref="G4:G59" si="0">D4*E4+F4</f>
+      <c r="H4" s="45">
+        <f t="shared" ref="H4:H59" si="0">E4*F4+G4</f>
         <v>30.71</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" s="42" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="49">
+    <row r="5" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="55" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="41">
         <v>3</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="C5" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="D5" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="49">
+      <c r="E5" s="41">
         <v>3</v>
       </c>
-      <c r="E5" s="51">
+      <c r="F5" s="44">
         <v>1.05</v>
       </c>
-      <c r="F5" s="51">
+      <c r="G5" s="44">
         <v>1.55</v>
       </c>
-      <c r="G5" s="52">
+      <c r="H5" s="45">
         <f t="shared" si="0"/>
         <v>4.7</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="L5" s="46" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="1"/>
-      <c r="B6" s="11"/>
-      <c r="D6" s="16"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B6" s="1"/>
+      <c r="C6" s="11"/>
+      <c r="E6" s="16"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="F7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
+      <c r="E7" s="17"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="41">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="16">
+      <c r="E8" s="41">
         <v>2</v>
       </c>
-      <c r="E8" s="14">
+      <c r="F8" s="44">
         <v>6.11</v>
       </c>
-      <c r="F8" s="27">
+      <c r="G8" s="44">
         <v>1.74</v>
       </c>
-      <c r="G8" s="15">
+      <c r="H8" s="45">
         <f t="shared" si="0"/>
         <v>13.96</v>
       </c>
-      <c r="K8" s="43" t="s">
+      <c r="L8" s="46" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
+    <row r="9" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="41">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="16">
+      <c r="E9" s="41">
         <v>1</v>
       </c>
-      <c r="E9" s="14">
+      <c r="F9" s="44">
         <v>11.87</v>
       </c>
-      <c r="F9" s="27">
-        <v>0</v>
-      </c>
-      <c r="G9" s="15">
+      <c r="G9" s="44">
+        <v>0</v>
+      </c>
+      <c r="H9" s="45">
         <f t="shared" si="0"/>
         <v>11.87</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" s="46" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
+    <row r="10" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="41">
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="16">
+      <c r="E10" s="41">
         <v>3</v>
       </c>
-      <c r="E10" s="14">
+      <c r="F10" s="44">
         <v>7.28</v>
       </c>
-      <c r="F10" s="27">
+      <c r="G10" s="44">
         <v>1.74</v>
       </c>
-      <c r="G10" s="15">
+      <c r="H10" s="45">
         <f t="shared" si="0"/>
         <v>23.58</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" s="42" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
+    <row r="11" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="48" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="47">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="16">
+      <c r="E11" s="47">
         <v>2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="F11" s="49">
         <v>8.4600000000000009</v>
       </c>
-      <c r="F11" s="27">
+      <c r="G11" s="49">
         <v>1.74</v>
       </c>
-      <c r="G11" s="15">
+      <c r="H11" s="50">
         <f t="shared" si="0"/>
         <v>18.66</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" s="51" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
+    <row r="12" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="41">
         <v>9</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="16">
+      <c r="E12" s="41">
         <v>2</v>
       </c>
-      <c r="E12" s="14">
+      <c r="F12" s="44">
         <v>7.63</v>
       </c>
-      <c r="F12" s="27">
+      <c r="G12" s="44">
         <v>1.74</v>
       </c>
-      <c r="G12" s="15">
+      <c r="H12" s="45">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" s="42" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
+    <row r="13" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="48" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="47">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="16">
+      <c r="E13" s="47">
         <v>2</v>
       </c>
-      <c r="E13" s="14">
+      <c r="F13" s="49">
         <v>7.63</v>
       </c>
-      <c r="F13" s="27">
+      <c r="G13" s="49">
         <v>1.74</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H13" s="50">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" s="48" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="54">
+    <row r="14" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="47">
         <v>11</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="C14" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="D14" s="54">
+      <c r="E14" s="47">
         <v>16</v>
       </c>
-      <c r="E14" s="56">
+      <c r="F14" s="49">
         <v>6.46</v>
       </c>
-      <c r="F14" s="56">
-        <v>0</v>
-      </c>
-      <c r="G14" s="57">
-        <f>E14+F14</f>
+      <c r="G14" s="49">
+        <v>0</v>
+      </c>
+      <c r="H14" s="50">
+        <f>F14+G14</f>
         <v>6.46</v>
       </c>
-      <c r="K14" s="55" t="s">
+      <c r="L14" s="51" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="45" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="44">
+    <row r="15" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="36">
         <v>12</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="C15" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="D15" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="44">
+      <c r="E15" s="36">
         <v>4</v>
       </c>
-      <c r="E15" s="46">
+      <c r="F15" s="38">
         <v>3.68</v>
       </c>
-      <c r="F15" s="46">
+      <c r="G15" s="38">
         <v>4.96</v>
       </c>
-      <c r="G15" s="47">
-        <f>E15+F15</f>
+      <c r="H15" s="39">
+        <f>F15+G15</f>
         <v>8.64</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="L15" s="40" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
+    <row r="16" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" s="47">
         <v>13</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="16">
+      <c r="E16" s="47">
         <v>4</v>
       </c>
-      <c r="E16" s="14">
+      <c r="F16" s="49">
         <f>1.7/4</f>
         <v>0.42499999999999999</v>
       </c>
-      <c r="F16" s="27">
+      <c r="G16" s="49">
         <v>1.37</v>
       </c>
-      <c r="G16" s="15">
+      <c r="H16" s="50">
         <f t="shared" si="0"/>
         <v>3.0700000000000003</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" s="51" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17" s="1">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="B17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="16">
+      <c r="E17" s="16">
         <v>2</v>
       </c>
-      <c r="E17" s="14">
+      <c r="F17" s="14">
         <v>0.23</v>
       </c>
-      <c r="F17" s="27">
-        <v>0</v>
-      </c>
-      <c r="G17" s="15">
+      <c r="G17" s="26">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" s="1">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D18" s="16">
+      <c r="E18" s="16">
         <v>1</v>
       </c>
-      <c r="E18" s="14">
+      <c r="F18" s="14">
         <v>0.46</v>
       </c>
-      <c r="F18" s="27">
-        <v>0</v>
-      </c>
-      <c r="G18" s="15">
+      <c r="G18" s="26">
+        <v>0</v>
+      </c>
+      <c r="H18" s="15">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" s="35" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19" s="1"/>
-      <c r="B19" s="11"/>
-      <c r="D19" s="16"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B19" s="1"/>
+      <c r="C19" s="11"/>
+      <c r="E19" s="16"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="F20" s="29"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
+      <c r="E20" s="18"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" s="47">
         <v>16</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="16">
+      <c r="E21" s="47">
         <v>8</v>
       </c>
-      <c r="E21" s="38">
+      <c r="F21" s="65">
         <v>1.84</v>
       </c>
-      <c r="F21" s="37">
-        <v>0</v>
-      </c>
-      <c r="G21" s="40">
-        <f>E21+F21</f>
+      <c r="G21" s="65">
+        <v>0</v>
+      </c>
+      <c r="H21" s="66">
+        <f>F21+G21</f>
         <v>1.84</v>
       </c>
-      <c r="K21" s="39" t="s">
+      <c r="L21" s="67" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
+    <row r="22" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="47">
         <v>17</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="D22" s="16">
+      <c r="E22" s="47">
         <v>12</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="40"/>
-      <c r="K22" s="39"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="66"/>
+      <c r="L22" s="68"/>
+    </row>
+    <row r="23" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="47">
         <v>18</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="16">
+      <c r="E23" s="47">
         <v>8</v>
       </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="40"/>
-      <c r="K23" s="39"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="66"/>
+      <c r="L23" s="68"/>
+    </row>
+    <row r="24" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="47">
         <v>19</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="16">
+      <c r="E24" s="47">
         <v>2</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="40"/>
-      <c r="K24" s="39"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25" s="1">
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="66"/>
+      <c r="L24" s="68"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="1">
         <v>20</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="16">
+      <c r="E25" s="16">
         <v>2</v>
       </c>
-      <c r="E25" s="41">
+      <c r="F25" s="63">
         <v>5.75</v>
       </c>
-      <c r="F25" s="42">
-        <v>0</v>
-      </c>
-      <c r="G25" s="40">
-        <f>E25+F25</f>
+      <c r="G25" s="64">
+        <v>0</v>
+      </c>
+      <c r="H25" s="62">
+        <f>F25+G25</f>
         <v>5.75</v>
       </c>
-      <c r="K25" s="39" t="s">
+      <c r="L25" s="61" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A26" s="1">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" s="48"/>
+      <c r="B26" s="1">
         <v>21</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="16">
+      <c r="E26" s="16">
         <v>19</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="40"/>
-      <c r="K26" s="39"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" s="1">
+      <c r="F26" s="63"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="62"/>
+      <c r="L26" s="60"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="48"/>
+      <c r="B27" s="1">
         <v>22</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="16">
+      <c r="E27" s="16">
         <v>10</v>
       </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="40"/>
-      <c r="K27" s="39"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
+      <c r="F27" s="63"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="62"/>
+      <c r="L27" s="60"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" s="48"/>
+      <c r="B28" s="1">
         <v>23</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="16">
+      <c r="E28" s="16">
         <v>12</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="40"/>
-      <c r="K28" s="39"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A29" s="1">
+      <c r="F28" s="63"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="62"/>
+      <c r="L28" s="60"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" s="48"/>
+      <c r="B29" s="1">
         <v>24</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="16">
+      <c r="E29" s="16">
         <v>4</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="40"/>
-      <c r="K29" s="39"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A30" s="1">
+      <c r="F29" s="63"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="62"/>
+      <c r="L29" s="60"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="42"/>
+      <c r="B30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="16">
+      <c r="E30" s="16">
         <v>98</v>
       </c>
-      <c r="E30" s="14">
+      <c r="F30" s="14">
         <v>6.29</v>
       </c>
-      <c r="F30" s="27">
-        <v>0</v>
-      </c>
-      <c r="G30" s="15">
-        <f>E30+F30</f>
+      <c r="G30" s="26">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15">
+        <f>F30+G30</f>
         <v>6.29</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" s="42"/>
+      <c r="B31" s="1">
         <v>26</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>154</v>
       </c>
-      <c r="D31" s="16">
+      <c r="E31" s="16">
         <v>4</v>
       </c>
-      <c r="E31" s="41">
+      <c r="F31" s="63">
         <v>6.48</v>
       </c>
-      <c r="F31" s="42">
-        <v>0</v>
-      </c>
-      <c r="G31" s="36">
-        <f>E31+F31</f>
+      <c r="G31" s="64">
+        <v>0</v>
+      </c>
+      <c r="H31" s="57">
+        <f>F31+G31</f>
         <v>6.48</v>
       </c>
-      <c r="K31" s="39" t="s">
+      <c r="L31" s="61" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A32" s="1">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A32" s="42"/>
+      <c r="B32" s="1">
         <v>27</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="C32" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="16">
+      <c r="E32" s="16">
         <v>2</v>
       </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="36"/>
-      <c r="K32" s="39"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A33" s="1">
+      <c r="F32" s="63"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="57"/>
+      <c r="L32" s="60"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A33" s="42"/>
+      <c r="B33" s="1">
         <v>28</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="C33" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="16">
+      <c r="E33" s="16">
         <v>3</v>
       </c>
-      <c r="E33" s="14">
+      <c r="F33" s="14">
         <v>8.81</v>
       </c>
-      <c r="F33" s="27">
-        <v>0</v>
-      </c>
-      <c r="G33" s="15">
-        <f>E33+F33</f>
+      <c r="G33" s="26">
+        <v>0</v>
+      </c>
+      <c r="H33" s="15">
+        <f>F33+G33</f>
         <v>8.81</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" s="35" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A34" s="1">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A34" s="42"/>
+      <c r="B34" s="1">
         <v>29</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="C34" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="16">
+      <c r="E34" s="16">
         <v>18</v>
       </c>
-      <c r="E34" s="14">
+      <c r="F34" s="14">
         <v>2.33</v>
       </c>
-      <c r="F34" s="27">
-        <v>0</v>
-      </c>
-      <c r="G34" s="15">
-        <f>E34+F34</f>
+      <c r="G34" s="26">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15">
+        <f>F34+G34</f>
         <v>2.33</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A35" s="1">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A35" s="42"/>
+      <c r="B35" s="1">
         <v>30</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="16">
+      <c r="E35" s="16">
         <v>11</v>
       </c>
-      <c r="E35" s="14">
+      <c r="F35" s="14">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F35" s="27">
-        <v>0</v>
-      </c>
-      <c r="G35" s="15">
-        <f>E35+F35</f>
+      <c r="G35" s="26">
+        <v>0</v>
+      </c>
+      <c r="H35" s="15">
+        <f>F35+G35</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A36" s="42"/>
+      <c r="B36" s="1">
         <v>31</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="16">
+      <c r="E36" s="16">
         <v>13</v>
       </c>
-      <c r="E36" s="14">
+      <c r="F36" s="14">
         <v>2.33</v>
       </c>
-      <c r="F36" s="27">
-        <v>0</v>
-      </c>
-      <c r="G36" s="15">
-        <f>E36+F36</f>
+      <c r="G36" s="26">
+        <v>0</v>
+      </c>
+      <c r="H36" s="15">
+        <f>F36+G36</f>
         <v>2.33</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A37" s="1">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37" s="42"/>
+      <c r="B37" s="1">
         <v>32</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="C37" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>131</v>
       </c>
-      <c r="D37" s="16">
+      <c r="E37" s="16">
         <v>9</v>
       </c>
-      <c r="E37" s="14">
+      <c r="F37" s="14">
         <v>0.47</v>
       </c>
-      <c r="F37" s="27">
-        <v>0</v>
-      </c>
-      <c r="G37" s="15">
+      <c r="G37" s="26">
+        <v>0</v>
+      </c>
+      <c r="H37" s="15">
         <f t="shared" si="0"/>
         <v>4.2299999999999995</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A38" s="1">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A38" s="42"/>
+      <c r="B38" s="1">
         <v>33</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="16">
+      <c r="E38" s="16">
         <v>2</v>
       </c>
-      <c r="E38" s="14">
+      <c r="F38" s="14">
         <v>0.48</v>
       </c>
-      <c r="F38" s="27">
-        <v>0</v>
-      </c>
-      <c r="G38" s="15">
+      <c r="G38" s="26">
+        <v>0</v>
+      </c>
+      <c r="H38" s="15">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A39" s="42"/>
+      <c r="B39" s="1">
         <v>34</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="16">
+      <c r="E39" s="16">
         <v>102</v>
       </c>
-      <c r="E39" s="14">
+      <c r="F39" s="14">
         <v>1.91</v>
       </c>
-      <c r="F39" s="27">
-        <v>0</v>
-      </c>
-      <c r="G39" s="15">
-        <f>E39+F39</f>
+      <c r="G39" s="26">
+        <v>0</v>
+      </c>
+      <c r="H39" s="15">
+        <f>F39+G39</f>
         <v>1.91</v>
       </c>
-      <c r="K39" s="43" t="s">
+      <c r="L39" s="35" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A40" s="42"/>
+      <c r="B40" s="1">
         <v>35</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="C40" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="16">
+      <c r="E40" s="16">
         <v>2</v>
       </c>
-      <c r="E40" s="38">
+      <c r="F40" s="59">
         <v>0.23</v>
       </c>
-      <c r="F40" s="37">
-        <v>0</v>
-      </c>
-      <c r="G40" s="36">
+      <c r="G40" s="58">
+        <v>0</v>
+      </c>
+      <c r="H40" s="57">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-      <c r="K40" s="39" t="s">
+      <c r="L40" s="60" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A41" s="1">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A41" s="42"/>
+      <c r="B41" s="1">
         <v>36</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>116</v>
       </c>
-      <c r="D41" s="16">
+      <c r="E41" s="16">
         <v>4</v>
       </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="36"/>
-      <c r="K41" s="39"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A42" s="1">
+      <c r="F41" s="59"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="57"/>
+      <c r="L41" s="60"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A42" s="42"/>
+      <c r="B42" s="1">
         <v>37</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="C42" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="16">
+      <c r="E42" s="16">
         <v>4</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="36"/>
-      <c r="K42" s="39"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A43" s="1">
+      <c r="F42" s="59"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="57"/>
+      <c r="L42" s="60"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A43" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" s="1">
         <v>38</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="C43" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="16">
+      <c r="E43" s="16">
         <v>12</v>
       </c>
-      <c r="E43" s="14">
+      <c r="F43" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="F43" s="27">
+      <c r="G43" s="26">
         <v>1.81</v>
       </c>
-      <c r="G43" s="15">
-        <f>E43+F43</f>
+      <c r="H43" s="15">
+        <f>F43+G43</f>
         <v>2.93</v>
       </c>
-      <c r="K43" s="43" t="s">
+      <c r="L43" s="35" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A44" s="1">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A44" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="B44" s="1">
         <v>39</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="C44" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="16">
+      <c r="E44" s="16">
         <v>14</v>
       </c>
-      <c r="E44" s="14">
+      <c r="F44" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="F44" s="27">
+      <c r="G44" s="26">
         <v>1.81</v>
       </c>
-      <c r="G44" s="15">
-        <f>E44+F44</f>
+      <c r="H44" s="15">
+        <f>F44+G44</f>
         <v>2.93</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A45" s="1"/>
-      <c r="B45" s="11"/>
-      <c r="D45" s="16"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="15"/>
-    </row>
-    <row r="46" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="5" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B45" s="1"/>
+      <c r="C45" s="11"/>
+      <c r="E45" s="16"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="15"/>
+    </row>
+    <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="19"/>
-      <c r="F46" s="30"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A47" s="1">
+      <c r="E46" s="19"/>
+      <c r="G46" s="29"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B47" s="1">
         <v>40</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="C47" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="16">
+      <c r="E47" s="16">
         <v>2</v>
       </c>
-      <c r="E47" s="14">
+      <c r="F47" s="14">
         <v>23.17</v>
       </c>
-      <c r="F47" s="27">
+      <c r="G47" s="26">
         <v>10.98</v>
       </c>
-      <c r="G47" s="15">
+      <c r="H47" s="15">
         <f t="shared" si="0"/>
         <v>57.320000000000007</v>
       </c>
-      <c r="K47" s="43" t="s">
+      <c r="L47" s="35" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A48" s="1">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B48" s="1">
         <v>41</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="16">
+      <c r="E48" s="16">
         <v>1</v>
       </c>
-      <c r="E48" s="14">
+      <c r="F48" s="14">
         <v>31.91</v>
       </c>
-      <c r="F48" s="27">
+      <c r="G48" s="26">
         <f>21.96/2</f>
         <v>10.98</v>
       </c>
-      <c r="G48" s="15">
+      <c r="H48" s="15">
         <f t="shared" si="0"/>
         <v>42.89</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A49" s="1">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A49" s="42"/>
+      <c r="B49" s="1">
         <v>42</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="C49" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="16">
+      <c r="E49" s="16">
         <v>1</v>
       </c>
-      <c r="E49" s="14">
+      <c r="F49" s="14">
         <v>21.25</v>
       </c>
-      <c r="F49" s="27">
+      <c r="G49" s="26">
         <v>8.89</v>
       </c>
-      <c r="G49" s="15">
+      <c r="H49" s="15">
         <f t="shared" si="0"/>
         <v>30.14</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" s="35" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A50" s="1">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A50" s="42"/>
+      <c r="B50" s="1">
         <v>43</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="C50" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="16">
+      <c r="E50" s="16">
         <v>1</v>
       </c>
-      <c r="E50" s="14">
+      <c r="F50" s="14">
         <v>12.61</v>
       </c>
-      <c r="F50" s="27">
+      <c r="G50" s="26">
         <v>0.79</v>
       </c>
-      <c r="G50" s="15">
+      <c r="H50" s="15">
         <f t="shared" si="0"/>
         <v>13.399999999999999</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A51" s="1"/>
-      <c r="B51" s="11"/>
-      <c r="D51" s="16"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="15"/>
-    </row>
-    <row r="52" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="6" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B51" s="1"/>
+      <c r="C51" s="11"/>
+      <c r="E51" s="16"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="15"/>
+    </row>
+    <row r="52" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="20"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A53" s="1">
+      <c r="E52" s="20"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B53" s="1">
         <v>44</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="C53" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="16">
+      <c r="E53" s="16">
         <v>1</v>
       </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="15">
+      <c r="F53" s="14"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A54" s="1">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B54" s="1">
         <v>45</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="C54" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D54" s="16">
+      <c r="E54" s="16">
         <v>1</v>
       </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="15">
+      <c r="F54" s="14"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A55" s="1">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B55" s="1">
         <v>46</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="C55" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D55" s="16">
+      <c r="E55" s="16">
         <v>1</v>
       </c>
-      <c r="E55" s="14"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="15">
+      <c r="F55" s="14"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A56" s="1">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B56" s="1">
         <v>47</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="C56" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D56" s="16">
+      <c r="E56" s="16">
         <v>1</v>
       </c>
-      <c r="E56" s="14"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="15">
+      <c r="F56" s="14"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A57" s="1">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B57" s="1">
         <v>48</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="C57" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D57" s="16">
+      <c r="E57" s="16">
         <v>1</v>
       </c>
-      <c r="E57" s="14"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="15">
+      <c r="F57" s="14"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A58" s="1">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B58" s="1">
         <v>49</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="C58" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D58" s="16">
+      <c r="E58" s="16">
         <v>1</v>
       </c>
-      <c r="E58" s="14"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="15">
+      <c r="F58" s="14"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A59" s="1">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B59" s="1">
         <v>50</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="C59" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D59" s="16">
+      <c r="E59" s="16">
         <v>1</v>
       </c>
-      <c r="E59" s="14"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="15">
+      <c r="F59" s="14"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A60" s="1"/>
-      <c r="B60" s="11"/>
-      <c r="D60" s="16"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="15"/>
-    </row>
-    <row r="61" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="7" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B60" s="1"/>
+      <c r="C60" s="11"/>
+      <c r="E60" s="16"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="15"/>
+    </row>
+    <row r="61" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="D61" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="E61" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F61" s="32"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A62" s="1">
+      <c r="G61" s="31"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B62" s="1">
         <v>51</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="C62" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="16">
+      <c r="E62" s="16">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="E62" s="38">
+      <c r="F62" s="59">
         <v>25.61</v>
       </c>
-      <c r="F62" s="27">
-        <v>0</v>
-      </c>
-      <c r="G62" s="15">
-        <f>D62*$E$62+F62</f>
+      <c r="G62" s="26">
+        <v>0</v>
+      </c>
+      <c r="H62" s="15">
+        <f>E62*$F$62+G62</f>
         <v>0.84513000000000005</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A63" s="1">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B63" s="1">
         <v>52</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="C63" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>33</v>
       </c>
-      <c r="D63" s="22">
+      <c r="E63" s="22">
         <v>0.01</v>
       </c>
-      <c r="E63" s="38"/>
-      <c r="F63" s="27">
-        <v>0</v>
-      </c>
-      <c r="G63" s="15">
-        <f>D63*$E$62+F63</f>
+      <c r="F63" s="59"/>
+      <c r="G63" s="26">
+        <v>0</v>
+      </c>
+      <c r="H63" s="15">
+        <f>E63*$F$62+G63</f>
         <v>0.25609999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A64" s="1">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B64" s="1">
         <v>53</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="C64" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>36</v>
       </c>
-      <c r="D64" s="16">
+      <c r="E64" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E64" s="38"/>
-      <c r="F64" s="27">
-        <v>0</v>
-      </c>
-      <c r="G64" s="15">
-        <f>D64*$E$62+F64</f>
+      <c r="F64" s="59"/>
+      <c r="G64" s="26">
+        <v>0</v>
+      </c>
+      <c r="H64" s="15">
+        <f>E64*$F$62+G64</f>
         <v>0.20488000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A65" s="1">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B65" s="1">
         <v>54</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="C65" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>37</v>
       </c>
-      <c r="D65" s="16">
+      <c r="E65" s="16">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E65" s="38"/>
-      <c r="F65" s="27">
-        <v>0</v>
-      </c>
-      <c r="G65" s="15">
-        <f t="shared" ref="G65:G77" si="1">D65*$E$62+F65</f>
+      <c r="F65" s="59"/>
+      <c r="G65" s="26">
+        <v>0</v>
+      </c>
+      <c r="H65" s="15">
+        <f t="shared" ref="H65:H77" si="1">E65*$F$62+G65</f>
         <v>0.23048999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A66" s="1">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B66" s="1">
         <v>55</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="C66" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="16">
+      <c r="E66" s="16">
         <v>1.2E-2</v>
       </c>
-      <c r="E66" s="38"/>
-      <c r="F66" s="27">
-        <v>0</v>
-      </c>
-      <c r="G66" s="15">
+      <c r="F66" s="59"/>
+      <c r="G66" s="26">
+        <v>0</v>
+      </c>
+      <c r="H66" s="15">
         <f t="shared" si="1"/>
         <v>0.30731999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A67" s="1">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B67" s="1">
         <v>56</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="C67" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="16">
+      <c r="E67" s="16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E67" s="38"/>
-      <c r="F67" s="27">
-        <v>0</v>
-      </c>
-      <c r="G67" s="15">
+      <c r="F67" s="59"/>
+      <c r="G67" s="26">
+        <v>0</v>
+      </c>
+      <c r="H67" s="15">
         <f t="shared" si="1"/>
         <v>0.10244</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A68" s="1">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B68" s="1">
         <v>57</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="C68" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="16">
+      <c r="E68" s="16">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E68" s="38"/>
-      <c r="F68" s="27">
-        <v>0</v>
-      </c>
-      <c r="G68" s="15">
+      <c r="F68" s="59"/>
+      <c r="G68" s="26">
+        <v>0</v>
+      </c>
+      <c r="H68" s="15">
         <f t="shared" si="1"/>
         <v>0.64024999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A69" s="1">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B69" s="1">
         <v>58</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="C69" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="16">
+      <c r="E69" s="16">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E69" s="38"/>
-      <c r="F69" s="27">
-        <v>0</v>
-      </c>
-      <c r="G69" s="15">
+      <c r="F69" s="59"/>
+      <c r="G69" s="26">
+        <v>0</v>
+      </c>
+      <c r="H69" s="15">
         <f t="shared" si="1"/>
         <v>1.6902600000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A70" s="1">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B70" s="1">
         <v>59</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="C70" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>50</v>
       </c>
-      <c r="D70" s="16">
+      <c r="E70" s="16">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E70" s="38"/>
-      <c r="F70" s="27">
-        <v>0</v>
-      </c>
-      <c r="G70" s="15">
+      <c r="F70" s="59"/>
+      <c r="G70" s="26">
+        <v>0</v>
+      </c>
+      <c r="H70" s="15">
         <f t="shared" si="1"/>
         <v>0.43537000000000003</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A71" s="1">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B71" s="1">
         <v>60</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="C71" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>51</v>
       </c>
-      <c r="D71" s="16">
+      <c r="E71" s="16">
         <v>2.4E-2</v>
       </c>
-      <c r="E71" s="38"/>
-      <c r="F71" s="27">
-        <v>0</v>
-      </c>
-      <c r="G71" s="15">
+      <c r="F71" s="59"/>
+      <c r="G71" s="26">
+        <v>0</v>
+      </c>
+      <c r="H71" s="15">
         <f t="shared" si="1"/>
         <v>0.61463999999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A72" s="1">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B72" s="1">
         <v>61</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="C72" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>49</v>
       </c>
-      <c r="D72" s="16">
+      <c r="E72" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E72" s="38"/>
-      <c r="F72" s="27">
-        <v>0</v>
-      </c>
-      <c r="G72" s="15">
+      <c r="F72" s="59"/>
+      <c r="G72" s="26">
+        <v>0</v>
+      </c>
+      <c r="H72" s="15">
         <f t="shared" si="1"/>
         <v>7.6829999999999996E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A73" s="1">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B73" s="1">
         <v>62</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="C73" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>49</v>
       </c>
-      <c r="D73" s="16">
+      <c r="E73" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E73" s="38"/>
-      <c r="F73" s="27">
-        <v>0</v>
-      </c>
-      <c r="G73" s="15">
+      <c r="F73" s="59"/>
+      <c r="G73" s="26">
+        <v>0</v>
+      </c>
+      <c r="H73" s="15">
         <f t="shared" si="1"/>
         <v>7.6829999999999996E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A74" s="1">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B74" s="1">
         <v>63</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="C74" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>44</v>
       </c>
-      <c r="D74" s="16">
+      <c r="E74" s="16">
         <v>1.4E-2</v>
       </c>
-      <c r="E74" s="38"/>
-      <c r="F74" s="27">
-        <v>0</v>
-      </c>
-      <c r="G74" s="15">
+      <c r="F74" s="59"/>
+      <c r="G74" s="26">
+        <v>0</v>
+      </c>
+      <c r="H74" s="15">
         <f t="shared" si="1"/>
         <v>0.35854000000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A75" s="1">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B75" s="1">
         <v>64</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="C75" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>43</v>
       </c>
-      <c r="D75" s="16">
+      <c r="E75" s="16">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E75" s="38"/>
-      <c r="F75" s="27">
-        <v>0</v>
-      </c>
-      <c r="G75" s="15">
+      <c r="F75" s="59"/>
+      <c r="G75" s="26">
+        <v>0</v>
+      </c>
+      <c r="H75" s="15">
         <f t="shared" si="1"/>
         <v>0.33293</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A76" s="1">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B76" s="1">
         <v>65</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="C76" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>42</v>
       </c>
-      <c r="D76" s="16">
+      <c r="E76" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E76" s="38"/>
-      <c r="F76" s="27">
-        <v>0</v>
-      </c>
-      <c r="G76" s="15">
+      <c r="F76" s="59"/>
+      <c r="G76" s="26">
+        <v>0</v>
+      </c>
+      <c r="H76" s="15">
         <f t="shared" si="1"/>
         <v>0.20488000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A77" s="1">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B77" s="1">
         <v>66</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="C77" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>42</v>
       </c>
-      <c r="D77" s="16">
+      <c r="E77" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E77" s="38"/>
-      <c r="F77" s="27">
-        <v>0</v>
-      </c>
-      <c r="G77" s="15">
+      <c r="F77" s="59"/>
+      <c r="G77" s="26">
+        <v>0</v>
+      </c>
+      <c r="H77" s="15">
         <f t="shared" si="1"/>
         <v>0.20488000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A78" s="1"/>
-      <c r="B78" s="11"/>
-      <c r="D78" s="16"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="15"/>
-    </row>
-    <row r="79" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="9" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B78" s="1"/>
+      <c r="C78" s="11"/>
+      <c r="E78" s="16"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="15"/>
+    </row>
+    <row r="79" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B79" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D79" s="23"/>
-      <c r="F79" s="33"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A80" s="1">
+      <c r="E79" s="23"/>
+      <c r="G79" s="32"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A80" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="B80" s="1">
         <v>67</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="C80" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>174</v>
       </c>
-      <c r="D80" s="16">
+      <c r="E80" s="16">
         <v>1</v>
       </c>
-      <c r="E80" s="14">
+      <c r="F80" s="14">
         <v>0.48</v>
       </c>
-      <c r="F80" s="27">
-        <v>0</v>
-      </c>
-      <c r="G80" s="15">
-        <f t="shared" ref="G80:G125" si="2">D80*E80+F80</f>
+      <c r="G80" s="26">
+        <v>0</v>
+      </c>
+      <c r="H80" s="15">
+        <f t="shared" ref="H80:H125" si="2">E80*F80+G80</f>
         <v>0.48</v>
       </c>
-      <c r="K80" t="s">
+      <c r="L80" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A81" s="1">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A81" s="42"/>
+      <c r="B81" s="1">
         <v>68</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="C81" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D81" s="16">
+      <c r="E81" s="16">
         <v>1</v>
       </c>
-      <c r="E81" s="14">
+      <c r="F81" s="14">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F81" s="27">
+      <c r="G81" s="26">
         <v>1.21</v>
       </c>
-      <c r="G81" s="15">
+      <c r="H81" s="15">
         <f t="shared" si="2"/>
         <v>2.3200000000000003</v>
       </c>
-      <c r="K81" t="s">
+      <c r="L81" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A82" s="1">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A82" s="69" t="s">
+        <v>248</v>
+      </c>
+      <c r="B82" s="1">
         <v>69</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="C82" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="16">
+      <c r="E82" s="16">
         <v>1</v>
       </c>
-      <c r="E82" s="14">
-        <f>73.76-F82</f>
+      <c r="F82" s="14">
+        <f>73.76-G82</f>
         <v>73.760000000000005</v>
       </c>
-      <c r="F82" s="27">
-        <v>0</v>
-      </c>
-      <c r="G82" s="15">
+      <c r="G82" s="26">
+        <v>0</v>
+      </c>
+      <c r="H82" s="15">
         <f t="shared" si="2"/>
         <v>73.760000000000005</v>
       </c>
-      <c r="K82" t="s">
+      <c r="L82" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A83" s="1">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A83" s="69" t="s">
+        <v>249</v>
+      </c>
+      <c r="B83" s="1">
         <v>70</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="C83" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D83" s="16">
+      <c r="E83" s="16">
         <v>1</v>
       </c>
-      <c r="E83" s="14">
+      <c r="F83" s="14">
         <v>1.23</v>
       </c>
-      <c r="F83" s="27">
+      <c r="G83" s="26">
         <v>1.23</v>
       </c>
-      <c r="G83" s="15">
+      <c r="H83" s="15">
         <f t="shared" si="2"/>
         <v>2.46</v>
       </c>
-      <c r="K83" t="s">
+      <c r="L83" s="35" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A84" s="1">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A84" s="56"/>
+      <c r="B84" s="1">
         <v>71</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="C84" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>83</v>
       </c>
-      <c r="D84" s="16">
+      <c r="E84" s="16">
         <v>2</v>
       </c>
-      <c r="E84" s="14">
+      <c r="F84" s="14">
         <v>0.23</v>
       </c>
-      <c r="F84" s="27">
-        <v>0</v>
-      </c>
-      <c r="G84" s="15">
+      <c r="G84" s="26">
+        <v>0</v>
+      </c>
+      <c r="H84" s="15">
         <f t="shared" si="2"/>
         <v>0.46</v>
       </c>
-      <c r="K84" t="s">
+      <c r="L84" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A85" s="1">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A85" s="56"/>
+      <c r="B85" s="1">
         <v>72</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="C85" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>83</v>
       </c>
-      <c r="D85" s="16">
+      <c r="E85" s="16">
         <v>2</v>
       </c>
-      <c r="E85" s="14">
+      <c r="F85" s="14">
         <v>0.71</v>
       </c>
-      <c r="F85" s="27">
+      <c r="G85" s="26">
         <v>0.64</v>
       </c>
-      <c r="G85" s="15">
+      <c r="H85" s="15">
         <f t="shared" si="2"/>
         <v>2.06</v>
       </c>
-      <c r="K85" t="s">
+      <c r="L85" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A86" s="1">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A86" s="56"/>
+      <c r="B86" s="1">
         <v>73</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="C86" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>88</v>
       </c>
-      <c r="D86" s="16">
+      <c r="E86" s="16">
         <v>6</v>
       </c>
-      <c r="E86" s="14">
+      <c r="F86" s="14">
         <v>0.85</v>
       </c>
-      <c r="F86" s="27">
+      <c r="G86" s="26">
         <v>0.64</v>
       </c>
-      <c r="G86" s="15">
+      <c r="H86" s="15">
         <f t="shared" si="2"/>
         <v>5.7399999999999993</v>
       </c>
-      <c r="K86" t="s">
+      <c r="L86" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A87" s="1">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B87" s="1">
         <v>74</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="C87" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D87" s="16">
+      <c r="E87" s="16">
         <v>1</v>
       </c>
-      <c r="E87" s="14"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="15">
+      <c r="F87" s="14"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A88" s="1">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A88" s="56"/>
+      <c r="B88" s="1">
         <v>75</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="C88" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>86</v>
       </c>
-      <c r="D88" s="16">
+      <c r="E88" s="16">
         <v>3</v>
       </c>
-      <c r="E88" s="14">
+      <c r="F88" s="14">
         <v>1.28</v>
       </c>
-      <c r="F88" s="27">
+      <c r="G88" s="26">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G88" s="15">
+      <c r="H88" s="15">
         <f t="shared" si="2"/>
         <v>4.96</v>
       </c>
-      <c r="K88" t="s">
+      <c r="L88" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A89" s="1">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A89" s="42"/>
+      <c r="B89" s="1">
         <v>76</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="C89" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>94</v>
       </c>
-      <c r="D89" s="16">
+      <c r="E89" s="16">
         <v>1</v>
       </c>
-      <c r="E89" s="14">
+      <c r="F89" s="14">
         <v>0.43</v>
       </c>
-      <c r="F89" s="27">
+      <c r="G89" s="26">
         <v>0.91</v>
       </c>
-      <c r="G89" s="15">
+      <c r="H89" s="15">
         <f t="shared" si="2"/>
         <v>1.34</v>
       </c>
-      <c r="K89" t="s">
+      <c r="L89" s="35" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A90" s="1">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A90" s="71"/>
+      <c r="B90" s="1">
         <v>77</v>
       </c>
-      <c r="B90" s="11" t="s">
+      <c r="C90" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>108</v>
       </c>
-      <c r="D90" s="16">
+      <c r="E90" s="16">
         <v>1</v>
       </c>
-      <c r="E90" s="14">
+      <c r="F90" s="14">
         <v>22.63</v>
       </c>
-      <c r="F90" s="27">
-        <v>0</v>
-      </c>
-      <c r="G90" s="15">
+      <c r="G90" s="26">
+        <v>0</v>
+      </c>
+      <c r="H90" s="15">
         <f t="shared" si="2"/>
         <v>22.63</v>
       </c>
-      <c r="K90" t="s">
+      <c r="L90" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A91" s="1">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A91" s="53"/>
+      <c r="B91" s="1">
         <v>78</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="C91" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D91" s="16">
+      <c r="E91" s="16">
         <v>1</v>
       </c>
-      <c r="E91" s="14">
+      <c r="F91" s="14">
         <v>32.18</v>
       </c>
-      <c r="F91" s="27">
-        <v>0</v>
-      </c>
-      <c r="G91" s="15">
+      <c r="G91" s="26">
+        <v>0</v>
+      </c>
+      <c r="H91" s="15">
         <f t="shared" si="2"/>
         <v>32.18</v>
       </c>
-      <c r="K91" t="s">
+      <c r="L91" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A92" s="1">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A92" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="B92" s="1">
         <v>79</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="C92" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="D92" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="D92" s="16">
+      <c r="E92" s="16">
         <v>1</v>
       </c>
-      <c r="E92" s="14">
+      <c r="F92" s="14">
         <v>5.49</v>
       </c>
-      <c r="F92" s="27">
-        <v>0</v>
-      </c>
-      <c r="G92" s="15">
+      <c r="G92" s="26">
+        <v>0</v>
+      </c>
+      <c r="H92" s="15">
         <f t="shared" si="2"/>
         <v>5.49</v>
       </c>
-      <c r="K92" t="s">
+      <c r="L92" s="35" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A93" s="1">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A93" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="B93" s="1">
         <v>80</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="C93" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="D93" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D93" s="16">
+      <c r="E93" s="16">
         <v>1</v>
       </c>
-      <c r="E93" s="14">
+      <c r="F93" s="14">
         <v>4.54</v>
       </c>
-      <c r="F93" s="27">
+      <c r="G93" s="26">
         <v>5.66</v>
       </c>
-      <c r="G93" s="15">
+      <c r="H93" s="15">
         <f t="shared" si="2"/>
         <v>10.199999999999999</v>
       </c>
-      <c r="K93" t="s">
+      <c r="L93" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A94" s="1">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B94" s="1">
         <v>81</v>
       </c>
-      <c r="B94" s="11" t="s">
+      <c r="C94" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C94" s="12" t="s">
+      <c r="D94" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D94" s="16">
+      <c r="E94" s="16">
         <v>2</v>
       </c>
-      <c r="E94" s="14">
+      <c r="F94" s="14">
         <v>56.6</v>
       </c>
-      <c r="F94" s="27">
-        <v>0</v>
-      </c>
-      <c r="G94" s="15">
+      <c r="G94" s="26">
+        <v>0</v>
+      </c>
+      <c r="H94" s="15">
         <f t="shared" si="2"/>
         <v>113.2</v>
       </c>
-      <c r="K94" t="s">
+      <c r="L94" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A95" s="1">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A95" s="42"/>
+      <c r="B95" s="1">
         <v>82</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="C95" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C95" s="12" t="s">
+      <c r="D95" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D95" s="16">
+      <c r="E95" s="16">
         <v>1</v>
       </c>
-      <c r="E95" s="14">
+      <c r="F95" s="14">
         <v>1.1200000000000001</v>
       </c>
-      <c r="F95" s="27">
+      <c r="G95" s="26">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G95" s="15">
+      <c r="H95" s="15">
         <f t="shared" si="2"/>
         <v>1.7000000000000002</v>
       </c>
-      <c r="K95" t="s">
+      <c r="L95" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A96" s="1">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A96" s="42"/>
+      <c r="B96" s="1">
         <v>83</v>
       </c>
-      <c r="B96" s="11" t="s">
+      <c r="C96" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="D96" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D96" s="16">
+      <c r="E96" s="16">
         <v>1</v>
       </c>
-      <c r="E96" s="14">
+      <c r="F96" s="14">
         <v>0.69</v>
       </c>
-      <c r="F96" s="27">
+      <c r="G96" s="26">
         <v>2.69</v>
       </c>
-      <c r="G96" s="15">
+      <c r="H96" s="15">
         <f t="shared" si="2"/>
         <v>3.38</v>
       </c>
-      <c r="K96" t="s">
+      <c r="L96" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A97" s="1">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A97" s="42"/>
+      <c r="B97" s="1">
         <v>84</v>
       </c>
-      <c r="B97" s="11" t="s">
+      <c r="C97" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C97" s="12"/>
-      <c r="D97" s="16">
+      <c r="D97" s="12"/>
+      <c r="E97" s="16">
         <v>6</v>
       </c>
-      <c r="E97" s="14">
+      <c r="F97" s="14">
         <v>2.21</v>
       </c>
-      <c r="F97" s="27">
-        <v>0</v>
-      </c>
-      <c r="G97" s="15">
-        <f>E97+F97</f>
+      <c r="G97" s="26">
+        <v>0</v>
+      </c>
+      <c r="H97" s="15">
+        <f>F97+G97</f>
         <v>2.21</v>
       </c>
-      <c r="K97" t="s">
+      <c r="L97" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A98" s="1"/>
-      <c r="B98" s="11"/>
-      <c r="D98" s="16"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="15"/>
-    </row>
-    <row r="99" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="8" t="s">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B98" s="1"/>
+      <c r="C98" s="11"/>
+      <c r="E98" s="16"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="15"/>
+    </row>
+    <row r="99" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B99" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D99" s="24"/>
-      <c r="F99" s="34"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A100" s="1">
+      <c r="E99" s="24"/>
+      <c r="G99" s="33"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A100" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="B100" s="1">
         <v>85</v>
       </c>
-      <c r="B100" s="11" t="s">
+      <c r="C100" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C100" s="12" t="s">
+      <c r="D100" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D100" s="16">
+      <c r="E100" s="16">
         <v>2</v>
       </c>
-      <c r="E100" s="38">
+      <c r="F100" s="59">
         <v>0.47</v>
       </c>
-      <c r="F100" s="37">
-        <v>0</v>
-      </c>
-      <c r="G100" s="40">
+      <c r="G100" s="58">
+        <v>0</v>
+      </c>
+      <c r="H100" s="62">
         <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
-      <c r="K100" s="39" t="s">
+      <c r="L100" s="61" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A101" s="1">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A101" s="48"/>
+      <c r="B101" s="1">
         <v>86</v>
       </c>
-      <c r="B101" s="11" t="s">
+      <c r="C101" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C101" s="12" t="s">
+      <c r="D101" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D101" s="16">
+      <c r="E101" s="16">
         <v>1</v>
       </c>
-      <c r="E101" s="38"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="40"/>
-      <c r="K101" s="39"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A102" s="1">
+      <c r="F101" s="59"/>
+      <c r="G101" s="58"/>
+      <c r="H101" s="62"/>
+      <c r="L101" s="60"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A102" s="48"/>
+      <c r="B102" s="1">
         <v>87</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="C102" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C102" s="12" t="s">
+      <c r="D102" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D102" s="16">
+      <c r="E102" s="16">
         <v>4</v>
       </c>
-      <c r="E102" s="38"/>
-      <c r="F102" s="37"/>
-      <c r="G102" s="40"/>
-      <c r="K102" s="39"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A103" s="1">
+      <c r="F102" s="59"/>
+      <c r="G102" s="58"/>
+      <c r="H102" s="62"/>
+      <c r="L102" s="60"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A103" s="48"/>
+      <c r="B103" s="1">
         <v>88</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="C103" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C103" s="12" t="s">
+      <c r="D103" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D103" s="16">
+      <c r="E103" s="16">
         <v>1</v>
       </c>
-      <c r="E103" s="38"/>
-      <c r="F103" s="37"/>
-      <c r="G103" s="40"/>
-      <c r="K103" s="39"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A104" s="1">
+      <c r="F103" s="59"/>
+      <c r="G103" s="58"/>
+      <c r="H103" s="62"/>
+      <c r="L103" s="60"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A104" s="48"/>
+      <c r="B104" s="1">
         <v>89</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="C104" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C104" s="12" t="s">
+      <c r="D104" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D104" s="16">
+      <c r="E104" s="16">
         <v>4</v>
       </c>
-      <c r="E104" s="38"/>
-      <c r="F104" s="37"/>
-      <c r="G104" s="40"/>
-      <c r="K104" s="39"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A105" s="1">
+      <c r="F104" s="59"/>
+      <c r="G104" s="58"/>
+      <c r="H104" s="62"/>
+      <c r="L104" s="60"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A105" s="48"/>
+      <c r="B105" s="1">
         <v>90</v>
       </c>
-      <c r="B105" s="11" t="s">
+      <c r="C105" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C105" s="12" t="s">
+      <c r="D105" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D105" s="16">
+      <c r="E105" s="16">
         <v>2</v>
       </c>
-      <c r="E105" s="38"/>
-      <c r="F105" s="37"/>
-      <c r="G105" s="40"/>
-      <c r="K105" s="39"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A106" s="1">
+      <c r="F105" s="59"/>
+      <c r="G105" s="58"/>
+      <c r="H105" s="62"/>
+      <c r="L105" s="60"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A106" s="48"/>
+      <c r="B106" s="1">
         <v>91</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="C106" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>149</v>
       </c>
-      <c r="D106" s="16">
+      <c r="E106" s="16">
         <v>1</v>
       </c>
-      <c r="E106" s="38"/>
-      <c r="F106" s="37"/>
-      <c r="G106" s="40"/>
-      <c r="K106" s="39"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A107" s="1">
+      <c r="F106" s="59"/>
+      <c r="G106" s="58"/>
+      <c r="H106" s="62"/>
+      <c r="L106" s="60"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A107" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="B107" s="1">
         <v>92</v>
       </c>
-      <c r="B107" s="11" t="s">
+      <c r="C107" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>109</v>
       </c>
-      <c r="D107" s="16">
+      <c r="E107" s="16">
         <v>2</v>
       </c>
-      <c r="E107" s="38">
+      <c r="F107" s="59">
         <v>3.28</v>
       </c>
-      <c r="F107" s="37">
-        <v>0</v>
-      </c>
-      <c r="G107" s="36">
+      <c r="G107" s="58">
+        <v>0</v>
+      </c>
+      <c r="H107" s="57">
         <f t="shared" si="2"/>
         <v>6.56</v>
       </c>
-      <c r="K107" s="39" t="s">
+      <c r="L107" s="61" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A108" s="1">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A108" s="48"/>
+      <c r="B108" s="1">
         <v>93</v>
       </c>
-      <c r="B108" s="11" t="s">
+      <c r="C108" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>110</v>
       </c>
-      <c r="D108" s="16">
+      <c r="E108" s="16">
         <v>1</v>
       </c>
-      <c r="E108" s="38"/>
-      <c r="F108" s="37"/>
-      <c r="G108" s="36"/>
-      <c r="K108" s="39"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A109" s="1">
+      <c r="F108" s="59"/>
+      <c r="G108" s="58"/>
+      <c r="H108" s="57"/>
+      <c r="L108" s="60"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A109" s="48"/>
+      <c r="B109" s="1">
         <v>94</v>
       </c>
-      <c r="B109" s="11" t="s">
+      <c r="C109" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>147</v>
       </c>
-      <c r="D109" s="16">
+      <c r="E109" s="16">
         <v>2</v>
       </c>
-      <c r="E109" s="38"/>
-      <c r="F109" s="37"/>
-      <c r="G109" s="36"/>
-      <c r="K109" s="39"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A110" s="1">
+      <c r="F109" s="59"/>
+      <c r="G109" s="58"/>
+      <c r="H109" s="57"/>
+      <c r="L109" s="60"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A110" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="B110" s="1">
         <v>95</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="C110" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>90</v>
       </c>
-      <c r="D110" s="16">
+      <c r="E110" s="16">
         <v>20</v>
       </c>
-      <c r="E110" s="14">
+      <c r="F110" s="14">
         <v>0.91</v>
       </c>
-      <c r="F110" s="27">
+      <c r="G110" s="26">
         <v>0.45</v>
       </c>
-      <c r="G110" s="15">
-        <f>E110+F110</f>
+      <c r="H110" s="15">
+        <f>F110+G110</f>
         <v>1.36</v>
       </c>
-      <c r="K110" t="s">
+      <c r="L110" s="35" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A111" s="1">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A111" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B111" s="1">
         <v>96</v>
       </c>
-      <c r="B111" s="11" t="s">
+      <c r="C111" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>152</v>
       </c>
-      <c r="D111" s="16">
+      <c r="E111" s="16">
         <v>3</v>
       </c>
-      <c r="E111" s="14">
+      <c r="F111" s="14">
         <v>0.61</v>
       </c>
-      <c r="F111" s="27">
+      <c r="G111" s="26">
         <v>0.45</v>
       </c>
-      <c r="G111" s="15">
+      <c r="H111" s="15">
         <f t="shared" si="2"/>
         <v>2.2800000000000002</v>
       </c>
-      <c r="K111" t="s">
+      <c r="L111" s="35" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A112" s="1">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A112" s="48"/>
+      <c r="B112" s="1">
         <v>97</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="C112" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
         <v>92</v>
       </c>
-      <c r="D112" s="16">
+      <c r="E112" s="16">
         <v>4</v>
       </c>
-      <c r="E112" s="14">
+      <c r="F112" s="14">
         <v>0.83</v>
       </c>
-      <c r="F112" s="27">
+      <c r="G112" s="26">
         <v>0.45</v>
       </c>
-      <c r="G112" s="15">
+      <c r="H112" s="15">
         <f t="shared" si="2"/>
         <v>3.77</v>
       </c>
-      <c r="K112" t="s">
+      <c r="L112" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A113" s="1">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A113" s="52"/>
+      <c r="B113" s="1">
         <v>98</v>
       </c>
-      <c r="B113" s="11" t="s">
+      <c r="C113" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
         <v>96</v>
       </c>
-      <c r="D113" s="16">
+      <c r="E113" s="16">
         <v>2</v>
       </c>
-      <c r="E113" s="14">
+      <c r="F113" s="14">
         <v>0.16</v>
       </c>
-      <c r="F113" s="27">
+      <c r="G113" s="26">
         <f>1.86/2</f>
         <v>0.93</v>
       </c>
-      <c r="G113" s="15">
-        <f>E113+F113</f>
+      <c r="H113" s="15">
+        <f>F113+G113</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="K113" t="s">
+      <c r="L113" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A114" s="1">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A114" s="52"/>
+      <c r="B114" s="1">
         <v>99</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="C114" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>96</v>
       </c>
-      <c r="D114" s="16">
+      <c r="E114" s="16">
         <v>2</v>
       </c>
-      <c r="E114" s="14">
+      <c r="F114" s="14">
         <v>0.11</v>
       </c>
-      <c r="F114" s="27">
+      <c r="G114" s="26">
         <v>0.93</v>
       </c>
-      <c r="G114" s="15">
+      <c r="H114" s="15">
         <f t="shared" si="2"/>
         <v>1.1500000000000001</v>
       </c>
-      <c r="K114" t="s">
+      <c r="L114" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A115" s="1">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A115" s="53"/>
+      <c r="B115" s="1">
         <v>100</v>
       </c>
-      <c r="B115" s="11" t="s">
+      <c r="C115" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>106</v>
       </c>
-      <c r="D115" s="16">
+      <c r="E115" s="16">
         <v>1</v>
       </c>
-      <c r="E115" s="14">
+      <c r="F115" s="14">
         <v>6.97</v>
       </c>
-      <c r="F115" s="27">
+      <c r="G115" s="26">
         <v>5.95</v>
       </c>
-      <c r="G115" s="15">
+      <c r="H115" s="15">
         <f t="shared" si="2"/>
         <v>12.92</v>
       </c>
-      <c r="K115" t="s">
+      <c r="L115" s="35" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A116" s="1">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A116" s="42"/>
+      <c r="B116" s="1">
         <v>101</v>
       </c>
-      <c r="B116" s="11" t="s">
+      <c r="C116" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>114</v>
       </c>
-      <c r="D116" s="16">
+      <c r="E116" s="16">
         <v>7</v>
       </c>
-      <c r="E116" s="38">
+      <c r="F116" s="59">
         <v>4.5</v>
       </c>
-      <c r="F116" s="37">
+      <c r="G116" s="58">
         <v>1.89</v>
       </c>
-      <c r="G116" s="36">
-        <f>E116+F116</f>
+      <c r="H116" s="57">
+        <f>F116+G116</f>
         <v>6.39</v>
       </c>
-      <c r="H116" s="35"/>
-      <c r="I116" s="35"/>
-      <c r="J116" s="35"/>
-      <c r="K116" s="39" t="s">
+      <c r="I116" s="34"/>
+      <c r="J116" s="34"/>
+      <c r="K116" s="34"/>
+      <c r="L116" s="60" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A117" s="1">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A117" s="42"/>
+      <c r="B117" s="1">
         <v>102</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="C117" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>113</v>
       </c>
-      <c r="D117" s="16">
+      <c r="E117" s="16">
         <v>1</v>
       </c>
-      <c r="E117" s="38"/>
-      <c r="F117" s="37"/>
-      <c r="G117" s="36"/>
-      <c r="H117" s="35"/>
-      <c r="I117" s="35"/>
-      <c r="J117" s="35"/>
-      <c r="K117" s="39"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A118" s="1">
+      <c r="F117" s="59"/>
+      <c r="G117" s="58"/>
+      <c r="H117" s="57"/>
+      <c r="I117" s="34"/>
+      <c r="J117" s="34"/>
+      <c r="K117" s="34"/>
+      <c r="L117" s="60"/>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A118" s="54" t="s">
+        <v>244</v>
+      </c>
+      <c r="B118" s="1">
         <v>103</v>
       </c>
-      <c r="B118" s="11" t="s">
+      <c r="C118" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>104</v>
       </c>
-      <c r="D118" s="16">
+      <c r="E118" s="16">
         <v>1</v>
       </c>
-      <c r="E118" s="14">
+      <c r="F118" s="14">
         <v>0.47</v>
       </c>
-      <c r="F118" s="27">
-        <v>0</v>
-      </c>
-      <c r="G118" s="15">
+      <c r="G118" s="26">
+        <v>0</v>
+      </c>
+      <c r="H118" s="15">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
-      <c r="K118" t="s">
+      <c r="L118" s="35" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A119" s="1">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A119" s="42"/>
+      <c r="B119" s="1">
         <v>104</v>
       </c>
-      <c r="B119" s="11" t="s">
+      <c r="C119" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>135</v>
       </c>
-      <c r="D119" s="16">
+      <c r="E119" s="16">
         <v>2</v>
       </c>
-      <c r="E119" s="14">
+      <c r="F119" s="14">
         <v>1.3</v>
       </c>
-      <c r="F119" s="27">
+      <c r="G119" s="26">
         <v>1.89</v>
       </c>
-      <c r="G119" s="15">
+      <c r="H119" s="15">
         <f t="shared" si="2"/>
         <v>4.49</v>
       </c>
-      <c r="K119" t="s">
+      <c r="L119" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A120" s="1">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A120" s="42"/>
+      <c r="B120" s="1">
         <v>105</v>
       </c>
-      <c r="B120" s="11" t="s">
+      <c r="C120" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>139</v>
       </c>
-      <c r="D120" s="16">
+      <c r="E120" s="16">
         <v>1</v>
       </c>
-      <c r="E120" s="14">
+      <c r="F120" s="14">
         <v>0.47</v>
       </c>
-      <c r="F120" s="27">
-        <v>0</v>
-      </c>
-      <c r="G120" s="15">
+      <c r="G120" s="26">
+        <v>0</v>
+      </c>
+      <c r="H120" s="15">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
-      <c r="K120" t="s">
+      <c r="L120" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A121" s="1">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A121" s="42"/>
+      <c r="B121" s="1">
         <v>106</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="C121" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
         <v>148</v>
       </c>
-      <c r="D121" s="16">
+      <c r="E121" s="16">
         <v>1</v>
       </c>
-      <c r="E121" s="14">
+      <c r="F121" s="14">
         <v>0.47</v>
       </c>
-      <c r="F121" s="27">
-        <v>0</v>
-      </c>
-      <c r="G121" s="15">
+      <c r="G121" s="26">
+        <v>0</v>
+      </c>
+      <c r="H121" s="15">
         <f t="shared" si="2"/>
         <v>0.47</v>
       </c>
-      <c r="K121" t="s">
+      <c r="L121" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A122" s="1">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A122" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="B122" s="1">
         <v>107</v>
       </c>
-      <c r="B122" s="11" t="s">
+      <c r="C122" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
         <v>140</v>
       </c>
-      <c r="D122" s="16">
+      <c r="E122" s="16">
         <v>2</v>
       </c>
-      <c r="E122" s="14">
+      <c r="F122" s="14">
         <v>1.72</v>
       </c>
-      <c r="F122" s="27">
+      <c r="G122" s="26">
         <v>2.15</v>
       </c>
-      <c r="G122" s="15">
+      <c r="H122" s="15">
         <f t="shared" si="2"/>
         <v>5.59</v>
       </c>
-      <c r="K122" t="s">
+      <c r="L122" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A123" s="1">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A123" s="42"/>
+      <c r="B123" s="1">
         <v>108</v>
       </c>
-      <c r="B123" s="11" t="s">
+      <c r="C123" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="16">
+      <c r="E123" s="16">
         <v>1</v>
       </c>
-      <c r="E123" s="14">
+      <c r="F123" s="14">
         <v>17.52</v>
       </c>
-      <c r="F123" s="27">
+      <c r="G123" s="26">
         <v>1.21</v>
       </c>
-      <c r="G123" s="15">
+      <c r="H123" s="15">
         <f t="shared" si="2"/>
         <v>18.73</v>
       </c>
-      <c r="K123" t="s">
+      <c r="L123" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A124" s="1">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A124" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" s="1">
         <v>109</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="C124" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>140</v>
       </c>
-      <c r="D124" s="16">
+      <c r="E124" s="16">
         <v>1</v>
       </c>
-      <c r="E124" s="14">
+      <c r="F124" s="14">
         <v>7.05</v>
       </c>
-      <c r="F124" s="27">
+      <c r="G124" s="26">
         <v>6.42</v>
       </c>
-      <c r="G124" s="15">
+      <c r="H124" s="15">
         <f t="shared" si="2"/>
         <v>13.469999999999999</v>
       </c>
-      <c r="K124" t="s">
+      <c r="L124" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A125" s="1">
+      <c r="M124" s="70" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A125" s="42"/>
+      <c r="B125" s="1">
         <v>110</v>
       </c>
-      <c r="B125" s="11" t="s">
+      <c r="C125" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D125" s="16">
+      <c r="E125" s="16">
         <v>1</v>
       </c>
-      <c r="E125" s="14">
+      <c r="F125" s="14">
         <v>0.75</v>
       </c>
-      <c r="F125" s="27">
+      <c r="G125" s="26">
         <v>5.07</v>
       </c>
-      <c r="G125" s="15">
+      <c r="H125" s="15">
         <f t="shared" si="2"/>
         <v>5.82</v>
       </c>
-      <c r="K125" t="s">
+      <c r="L125" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B126" s="11"/>
-      <c r="D126" s="16"/>
-      <c r="F126" s="11"/>
-      <c r="G126" s="15"/>
-    </row>
-    <row r="127" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A127" s="13" t="s">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C126" s="11"/>
+      <c r="E126" s="16"/>
+      <c r="G126" s="11"/>
+      <c r="H126" s="15"/>
+    </row>
+    <row r="127" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B127" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D127" s="25"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B128" s="11" t="s">
+      <c r="E127" s="25"/>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C128" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D128" s="16"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="11"/>
-      <c r="G128" s="15"/>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B129" s="11" t="s">
+      <c r="E128" s="16"/>
+      <c r="F128" s="14"/>
+      <c r="G128" s="11"/>
+      <c r="H128" s="15"/>
+    </row>
+    <row r="129" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C129" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D129" s="16"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="11"/>
-      <c r="G129" s="15"/>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B130" s="11" t="s">
+      <c r="E129" s="16"/>
+      <c r="F129" s="14"/>
+      <c r="G129" s="11"/>
+      <c r="H129" s="15"/>
+    </row>
+    <row r="130" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C130" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
         <v>162</v>
       </c>
-      <c r="D130" s="16"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="11"/>
-      <c r="G130" s="15"/>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B131" s="11" t="s">
+      <c r="E130" s="16"/>
+      <c r="F130" s="14"/>
+      <c r="G130" s="11"/>
+      <c r="H130" s="15"/>
+    </row>
+    <row r="131" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C131" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D131" s="16"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="15"/>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B132" s="11" t="s">
+      <c r="E131" s="16"/>
+      <c r="F131" s="14"/>
+      <c r="G131" s="11"/>
+      <c r="H131" s="15"/>
+    </row>
+    <row r="132" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C132" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="D132" s="16"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="11"/>
-      <c r="G132" s="15"/>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B133" s="11" t="s">
+      <c r="E132" s="16"/>
+      <c r="F132" s="14"/>
+      <c r="G132" s="11"/>
+      <c r="H132" s="15"/>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C133" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D133" s="16"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="11"/>
-      <c r="G133" s="15"/>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B134" s="11" t="s">
+      <c r="E133" s="16"/>
+      <c r="F133" s="14"/>
+      <c r="G133" s="11"/>
+      <c r="H133" s="15"/>
+    </row>
+    <row r="134" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C134" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D134" s="16"/>
-      <c r="E134" s="14"/>
-      <c r="F134" s="11"/>
-      <c r="G134" s="15"/>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B135" s="11"/>
-      <c r="D135" s="16"/>
-      <c r="F135" s="11"/>
-      <c r="G135" s="15"/>
+      <c r="E134" s="16"/>
+      <c r="F134" s="14"/>
+      <c r="G134" s="11"/>
+      <c r="H134" s="15"/>
+    </row>
+    <row r="135" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C135" s="11"/>
+      <c r="E135" s="16"/>
+      <c r="G135" s="11"/>
+      <c r="H135" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G32"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="L31:L32"/>
     <mergeCell ref="F21:F24"/>
     <mergeCell ref="G21:G24"/>
-    <mergeCell ref="K21:K24"/>
-    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="H25:H29"/>
     <mergeCell ref="G25:G29"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="K25:K29"/>
-    <mergeCell ref="E62:E77"/>
-    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="L25:L29"/>
+    <mergeCell ref="F62:F77"/>
     <mergeCell ref="F40:F42"/>
     <mergeCell ref="G40:G42"/>
-    <mergeCell ref="K40:K42"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="H116:H117"/>
     <mergeCell ref="G116:G117"/>
     <mergeCell ref="F116:F117"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="K116:K117"/>
-    <mergeCell ref="K100:K106"/>
+    <mergeCell ref="L116:L117"/>
+    <mergeCell ref="L100:L106"/>
+    <mergeCell ref="H100:H106"/>
     <mergeCell ref="G100:G106"/>
     <mergeCell ref="F100:F106"/>
-    <mergeCell ref="E100:E106"/>
-    <mergeCell ref="E107:E109"/>
     <mergeCell ref="F107:F109"/>
     <mergeCell ref="G107:G109"/>
-    <mergeCell ref="K107:K109"/>
+    <mergeCell ref="H107:H109"/>
+    <mergeCell ref="L107:L109"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K5" r:id="rId1" display="https://nl.aliexpress.com/item/1005001621676770.html?spm=a2g0o.productlist.main.45.7d113e71c5rpfz&amp;algo_pvid=0ba04a30-e339-455d-b8e5-7db9d5e80bba&amp;algo_exp_id=0ba04a30-e339-455d-b8e5-7db9d5e80bba-22&amp;pdp_npi=4%40dis%21EUR%210.91%210.73%21%21%210.96%21%21%40211b88ee16938682042218596e4ee1%2112000020026811115%21sea%21NL%210%21A&amp;curPageLogUid=FATsjuqZyCN2" xr:uid="{5FC40EA4-9144-4BAE-B64C-8868371DE487}"/>
-    <hyperlink ref="K15" r:id="rId2" display="https://nl.aliexpress.com/item/1005003681572582.html?spm=a2g0o.productlist.main.25.5ca63b58zzCfgb&amp;algo_pvid=e28b779e-7411-432f-84bb-55b8b368539a&amp;algo_exp_id=e28b779e-7411-432f-84bb-55b8b368539a-12&amp;pdp_npi=4%40dis%21EUR%214.71%214.61%21%21%214.94%21%21%40211b615316947243129446972eaa47%2112000026782305036%21sea%21NL%210%21AS&amp;curPageLogUid=B0LszgvKN7rm" xr:uid="{303B114A-933D-49E6-81BA-E90AE349D616}"/>
-    <hyperlink ref="K47" r:id="rId3" xr:uid="{DD6DBFEB-37F3-417C-B60F-B55B0A6D2385}"/>
-    <hyperlink ref="K43" r:id="rId4" xr:uid="{AAB92C9C-AA83-4BBF-A389-2BDBB1F76C6F}"/>
-    <hyperlink ref="K39" r:id="rId5" display="https://nl.aliexpress.com/item/32814359094.html?spm=a2g0o.productlist.main.1.71a75b4bs55PPO&amp;algo_pvid=3670bd18-bf23-4e76-b2d3-dc5f92dc157a&amp;algo_exp_id=3670bd18-bf23-4e76-b2d3-dc5f92dc157a-0&amp;pdp_npi=4%40dis%21EUR%213.18%210.47%21%21%213.34%21%21%4021038eda16947275404078740e14c3%2166498695474%21sea%21NL%210%21AS&amp;curPageLogUid=C1P3e9JiY4ac" xr:uid="{E9BB8966-4C12-472C-A2F4-119AC5EA7B57}"/>
-    <hyperlink ref="K8" r:id="rId6" display="https://nl.aliexpress.com/item/1005002537611699.html?spm=a2g0o.productlist.main.3.4a031ab0olaA8Y&amp;algo_pvid=1cb8bec3-2328-4782-988c-cffaef372e91&amp;algo_exp_id=1cb8bec3-2328-4782-988c-cffaef372e91-1&amp;pdp_npi=4%40dis%21EUR%217.49%215.98%21%21%217.88%21%21%40211b88f016938699631611766e6877%2112000021048744254%21sea%21NL%210%21A&amp;curPageLogUid=FJZzS7E2CY5k" xr:uid="{C55F262C-B92E-4639-A97A-7ACE54D4785D}"/>
+    <hyperlink ref="L5" r:id="rId1" display="https://nl.aliexpress.com/item/1005001621676770.html?spm=a2g0o.productlist.main.45.7d113e71c5rpfz&amp;algo_pvid=0ba04a30-e339-455d-b8e5-7db9d5e80bba&amp;algo_exp_id=0ba04a30-e339-455d-b8e5-7db9d5e80bba-22&amp;pdp_npi=4%40dis%21EUR%210.91%210.73%21%21%210.96%21%21%40211b88ee16938682042218596e4ee1%2112000020026811115%21sea%21NL%210%21A&amp;curPageLogUid=FATsjuqZyCN2" xr:uid="{5FC40EA4-9144-4BAE-B64C-8868371DE487}"/>
+    <hyperlink ref="L15" r:id="rId2" display="https://nl.aliexpress.com/item/1005003681572582.html?spm=a2g0o.productlist.main.25.5ca63b58zzCfgb&amp;algo_pvid=e28b779e-7411-432f-84bb-55b8b368539a&amp;algo_exp_id=e28b779e-7411-432f-84bb-55b8b368539a-12&amp;pdp_npi=4%40dis%21EUR%214.71%214.61%21%21%214.94%21%21%40211b615316947243129446972eaa47%2112000026782305036%21sea%21NL%210%21AS&amp;curPageLogUid=B0LszgvKN7rm" xr:uid="{303B114A-933D-49E6-81BA-E90AE349D616}"/>
+    <hyperlink ref="L47" r:id="rId3" xr:uid="{DD6DBFEB-37F3-417C-B60F-B55B0A6D2385}"/>
+    <hyperlink ref="L43" r:id="rId4" xr:uid="{AAB92C9C-AA83-4BBF-A389-2BDBB1F76C6F}"/>
+    <hyperlink ref="L39" r:id="rId5" display="https://nl.aliexpress.com/item/32814359094.html?spm=a2g0o.productlist.main.1.71a75b4bs55PPO&amp;algo_pvid=3670bd18-bf23-4e76-b2d3-dc5f92dc157a&amp;algo_exp_id=3670bd18-bf23-4e76-b2d3-dc5f92dc157a-0&amp;pdp_npi=4%40dis%21EUR%213.18%210.47%21%21%213.34%21%21%4021038eda16947275404078740e14c3%2166498695474%21sea%21NL%210%21AS&amp;curPageLogUid=C1P3e9JiY4ac" xr:uid="{E9BB8966-4C12-472C-A2F4-119AC5EA7B57}"/>
+    <hyperlink ref="L8" r:id="rId6" display="https://nl.aliexpress.com/item/1005002537611699.html?spm=a2g0o.productlist.main.3.4a031ab0olaA8Y&amp;algo_pvid=1cb8bec3-2328-4782-988c-cffaef372e91&amp;algo_exp_id=1cb8bec3-2328-4782-988c-cffaef372e91-1&amp;pdp_npi=4%40dis%21EUR%217.49%215.98%21%21%217.88%21%21%40211b88f016938699631611766e6877%2112000021048744254%21sea%21NL%210%21A&amp;curPageLogUid=FJZzS7E2CY5k" xr:uid="{C55F262C-B92E-4639-A97A-7ACE54D4785D}"/>
+    <hyperlink ref="L3" r:id="rId7" display="https://nl.aliexpress.com/item/1005005533260185.html?spm=a2g0o.productlist.main.21.d7193af5nTc0bL&amp;algo_pvid=0311f4ec-5321-4d68-99e3-2e47c6b58b74&amp;algo_exp_id=0311f4ec-5321-4d68-99e3-2e47c6b58b74-10&amp;pdp_npi=4%40dis%21EUR%2136.33%2135.24%21%21%2138.24%21%21%40211b88ef16938677846513431e329a%2112000033439717476%21sea%21NL%210%21A&amp;curPageLogUid=17Ds95Ps0tr9" xr:uid="{3CCB6FA8-93D8-4BE5-A244-796617DB4388}"/>
+    <hyperlink ref="L9" r:id="rId8" display="https://nl.aliexpress.com/item/1005002453496457.html?spm=a2g0o.productlist.main.51.1df46917MQxx1B&amp;algo_pvid=2cc73904-420a-4249-9133-c5c1c338129d&amp;algo_exp_id=2cc73904-420a-4249-9133-c5c1c338129d-25&amp;pdp_npi=4%40dis%21EUR%2119.64%2119.64%21%21%2120.67%21%21%4021038eda16938702597077618e5c7a%2112000020710616520%21sea%21NL%210%21A&amp;curPageLogUid=VMwzInqvGpVO" xr:uid="{35C0CBFA-61C3-4853-9829-14EB5D0BD66F}"/>
+    <hyperlink ref="L11" r:id="rId9" display="https://nl.aliexpress.com/item/1005002537611699.html?spm=a2g0o.productlist.main.3.4a031ab0olaA8Y&amp;algo_pvid=1cb8bec3-2328-4782-988c-cffaef372e91&amp;algo_exp_id=1cb8bec3-2328-4782-988c-cffaef372e91-1&amp;pdp_npi=4%40dis%21EUR%217.49%215.98%21%21%217.88%21%21%40211b88f016938699631611766e6877%2112000021048744254%21sea%21NL%210%21A&amp;curPageLogUid=FJZzS7E2CY5k" xr:uid="{C1AFE67B-6315-4C17-8397-D9C59150749A}"/>
+    <hyperlink ref="L14" r:id="rId10" display="https://nl.aliexpress.com/item/4000063076132.html?spm=a2g0o.productlist.main.25.7da814435etbcl&amp;algo_pvid=19aa6fcc-ced3-47ff-abb9-b12fac77b6bf&amp;algo_exp_id=19aa6fcc-ced3-47ff-abb9-b12fac77b6bf-12&amp;pdp_npi=4%40dis%21EUR%2112.20%216.46%21%21%2112.80%21%21%40211b615316947241743964861eaa47%2110000000161993707%21sea%21NL%210%21AS&amp;curPageLogUid=rLXXE8yB8w6T" xr:uid="{D1B86BA7-C134-4B3F-ACA9-C36871E47DEC}"/>
+    <hyperlink ref="L16" r:id="rId11" display="https://nl.aliexpress.com/item/1005005974742507.html?spm=a2g0o.productlist.main.45.7bac5dd5iFG5OJ&amp;algo_pvid=2046b9d0-bc3c-4736-8237-c5244236c177&amp;algo_exp_id=2046b9d0-bc3c-4736-8237-c5244236c177-22&amp;pdp_npi=4%40dis%21EUR%212.12%211.7%21%21%2116.27%21%21%40211b617a16939507018131128e6a33%2112000035130817674%21sea%21NL%210%21A&amp;curPageLogUid=S3SDvNti9Aof" xr:uid="{15E1B83F-87BD-4C52-97B6-DB1A82819AFD}"/>
+    <hyperlink ref="L18" r:id="rId12" display="https://nl.aliexpress.com/item/32933924674.html?spm=a2g0o.productlist.main.3.412c3931eQBrTb&amp;algo_pvid=9e3379fe-aa2c-4b70-85b0-87a244084bad&amp;algo_exp_id=9e3379fe-aa2c-4b70-85b0-87a244084bad-1&amp;pdp_npi=4%40dis%21EUR%210.70%210.46%21%21%210.74%21%21%40211b617a16939509787254501e6a33%2166224476012%21sea%21NL%210%21A&amp;curPageLogUid=FMX9X8mry7T9" xr:uid="{97F1DA47-E347-41EF-8A94-6B90258E4C84}"/>
+    <hyperlink ref="L21" r:id="rId13" display="https://nl.aliexpress.com/item/1005004833515587.html?spm=a2g0o.productlist.main.7.107a4abed7Lp4O&amp;algo_pvid=4e5c6b8d-3b2b-4882-8919-a36d85c2f3a4&amp;algo_exp_id=4e5c6b8d-3b2b-4882-8919-a36d85c2f3a4-3&amp;pdp_npi=4%40dis%21EUR%2113.46%211.84%21%21%2114.12%21%21%40211b88f116947270870846250efcfc%2112000030659841609%21sea%21NL%210%21AS&amp;curPageLogUid=aU9x01JDrid9" xr:uid="{8C8D25B0-5059-49C4-833D-14718D9D31CD}"/>
+    <hyperlink ref="L25" r:id="rId14" display="https://nl.aliexpress.com/item/1005004833515587.html?spm=a2g0o.productlist.main.7.107a4abed7Lp4O&amp;algo_pvid=4e5c6b8d-3b2b-4882-8919-a36d85c2f3a4&amp;algo_exp_id=4e5c6b8d-3b2b-4882-8919-a36d85c2f3a4-3&amp;pdp_npi=4%40dis%21EUR%2113.46%211.84%21%21%2114.12%21%21%40211b88f116947270870846250efcfc%2112000030659841609%21sea%21NL%210%21AS&amp;curPageLogUid=aU9x01JDrid9" xr:uid="{BEC1F674-9762-42F7-AE45-3253DB147CAC}"/>
+    <hyperlink ref="L31" r:id="rId15" display="https://nl.aliexpress.com/item/1005004129378778.html?spm=a2g0o.productlist.main.67.565d590atXPBRa&amp;algo_pvid=966ad033-4291-4696-85c4-f2033d81a041&amp;algo_exp_id=966ad033-4291-4696-85c4-f2033d81a041-33&amp;pdp_npi=4%40dis%21EUR%2112.58%213.99%21%21%2113.19%21%21%4021038eda16947278400843976e14c3%2112000028131816313%21sea%21NL%210%21AS&amp;curPageLogUid=WjhHm1uIKRo7" xr:uid="{AB31084D-41CF-4B02-A8BF-F4D842113AB0}"/>
+    <hyperlink ref="L33" r:id="rId16" display="https://nl.aliexpress.com/item/1005006034026066.html?spm=a2g0o.productlist.main.21.50886603JV22ri&amp;algo_pvid=5ac0b68b-b2eb-4c67-9b40-9e0facd0099b&amp;algo_exp_id=5ac0b68b-b2eb-4c67-9b40-9e0facd0099b-10&amp;pdp_npi=4%40dis%21EUR%218.59%218.59%21%21%2165.51%21%21%4021038eda16947276262111658e14c3%2112000035416757399%21sea%21NL%210%21AS&amp;curPageLogUid=zP4y8BI3SNzx" xr:uid="{32CE36C1-45F8-405E-BD17-924F8FA53C0F}"/>
+    <hyperlink ref="L49" r:id="rId17" xr:uid="{C686D0BE-525A-49BD-BB2E-EA291216792E}"/>
+    <hyperlink ref="L100" r:id="rId18" display="https://nl.aliexpress.com/item/1005004750475982.html?spm=a2g0o.productlist.main.15.33c626d9QHVmUn&amp;algo_pvid=e456ecd9-aba0-493f-9c6c-09f29dba53b9&amp;algo_exp_id=e456ecd9-aba0-493f-9c6c-09f29dba53b9-7&amp;pdp_npi=4%40dis%21EUR%214.10%210.47%21%21%214.32%21%21%40211b88ee16938711022977528e4ee0%2112000030335587229%21sea%21NL%210%21A&amp;curPageLogUid=rVN2Luqel4s8" xr:uid="{E4605858-B5DB-4411-976F-4D7F05DC1F70}"/>
+    <hyperlink ref="L107" r:id="rId19" display="https://nl.aliexpress.com/item/1005004750475982.html?spm=a2g0o.productlist.main.15.33c626d9QHVmUn&amp;algo_pvid=e456ecd9-aba0-493f-9c6c-09f29dba53b9&amp;algo_exp_id=e456ecd9-aba0-493f-9c6c-09f29dba53b9-7&amp;pdp_npi=4%40dis%21EUR%214.10%210.47%21%21%214.32%21%21%40211b88ee16938711022977528e4ee0%2112000030335587229%21sea%21NL%210%21A&amp;curPageLogUid=rVN2Luqel4s8" xr:uid="{83240247-77A9-4ABE-A083-B6D7F7D6D24C}"/>
+    <hyperlink ref="L110" r:id="rId20" display="https://nl.aliexpress.com/item/1005004300032921.html?spm=a2g0o.productlist.main.7.2de4185fYU0pdt&amp;algo_pvid=c988d294-ba9f-470b-b6c0-00092072a071&amp;algo_exp_id=c988d294-ba9f-470b-b6c0-00092072a071-3&amp;pdp_npi=4%40dis%21EUR%212.97%211.9%21%21%213.11%21%21%40211b5db216947249509028695e768d%2112000028678908419%21sea%21NL%210%21AS&amp;curPageLogUid=qhjVsdfWx3AP" xr:uid="{F6F1C24A-0AE2-4056-845F-5BD1EC002347}"/>
+    <hyperlink ref="L111" r:id="rId21" display="https://nl.aliexpress.com/item/1005004300032921.html?spm=a2g0o.productlist.main.7.2de4185fYU0pdt&amp;algo_pvid=c988d294-ba9f-470b-b6c0-00092072a071&amp;algo_exp_id=c988d294-ba9f-470b-b6c0-00092072a071-3&amp;pdp_npi=4%40dis%21EUR%212.97%211.9%21%21%213.11%21%21%40211b5db216947249509028695e768d%2112000028678908419%21sea%21NL%210%21AS&amp;curPageLogUid=qhjVsdfWx3AP" xr:uid="{F11764D2-57F0-44F1-A7FC-D7D9DFEACE61}"/>
+    <hyperlink ref="L83" r:id="rId22" display="https://nl.aliexpress.com/item/1005005793264636.html?pdp_npi=2%40dis%21EUR%21%E2%82%AC2%2C46%21%E2%82%AC1%2C23%21%21%21%21%21%40211b5e2b16938688945022418e9ea7%2112000034373780385%21btf&amp;_t=pvid%3A7ec7a95a-5d26-46b4-8dae-ac2173346fff&amp;spm=a2g0o.ppclist.product.mainProduct&amp;gatewayAdapt=glo2nld" xr:uid="{82B66CC5-C7CB-420C-8CE9-AD545C8B0AAF}"/>
+    <hyperlink ref="L89" r:id="rId23" display="https://nl.aliexpress.com/item/32803005422.html?spm=a2g0o.productlist.main.1.3e397860t4cqJR&amp;algo_pvid=0d3bf6ce-72ba-4bb5-8b94-153125c620c6&amp;algo_exp_id=0d3bf6ce-72ba-4bb5-8b94-153125c620c6-0&amp;pdp_npi=4%40dis%21EUR%210.48%210.43%21%21%210.51%21%21%40211b5e1f16938692423487198ef835%2164323132051%21sea%21NL%210%21A&amp;curPageLogUid=NExKTzmhwzbe" xr:uid="{1170F96B-D649-4A2C-A737-87DF1007A2A2}"/>
+    <hyperlink ref="L118" r:id="rId24" display="https://nl.aliexpress.com/item/1005004982855996.html?spm=a2g0o.productlist.main.13.2a7e34b4tX6oYt&amp;algo_pvid=d1a07258-b9e4-401e-9cff-f6ae64d56d05&amp;algo_exp_id=d1a07258-b9e4-401e-9cff-f6ae64d56d05-6&amp;pdp_npi=4%40dis%21EUR%211.53%210.47%21%21%211.60%21%21%4021038ed816947263048078897eb23d%2112000031234656880%21sea%21NL%210%21AS&amp;curPageLogUid=YRx9y1l6OZRt" xr:uid="{62EE5D5D-E2D2-45A8-BC29-D4FEE82DBE04}"/>
+    <hyperlink ref="L92" r:id="rId25" xr:uid="{BAEB2FD0-35E5-4E73-93BD-E2119B364C41}"/>
+    <hyperlink ref="L115" r:id="rId26" xr:uid="{71B38B44-CAEC-49E1-91E9-2B3FFD717800}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Frame + Fasteners
Having issues with smart fasteners feature
</commit_message>
<xml_diff>
--- a/BOM/BillOfMaterials.xlsx
+++ b/BOM/BillOfMaterials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reger\Documents\Project\Flex Delft Work\Open Hardware\Schistoscope\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279B9ED5-FF2F-4982-AEE1-EEA6DC6E0175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B86B21-9FAF-477E-B56E-B46AB9E0B039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{E17B2124-711C-4341-A725-6D6BA9A2AA94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="252">
   <si>
     <t>Name</t>
   </si>
@@ -787,6 +787,9 @@
   </si>
   <si>
     <t>Farnelll</t>
+  </si>
+  <si>
+    <t>Scope has CML100(?)</t>
   </si>
 </sst>
 </file>
@@ -986,7 +989,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1076,6 +1079,10 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1112,9 +1119,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1436,8 +1440,8 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1929,17 +1933,17 @@
       <c r="E21" s="47">
         <v>8</v>
       </c>
-      <c r="F21" s="65">
+      <c r="F21" s="69">
         <v>1.84</v>
       </c>
-      <c r="G21" s="65">
-        <v>0</v>
-      </c>
-      <c r="H21" s="66">
+      <c r="G21" s="69">
+        <v>0</v>
+      </c>
+      <c r="H21" s="70">
         <f>F21+G21</f>
         <v>1.84</v>
       </c>
-      <c r="L21" s="67" t="s">
+      <c r="L21" s="71" t="s">
         <v>220</v>
       </c>
     </row>
@@ -1956,10 +1960,10 @@
       <c r="E22" s="47">
         <v>12</v>
       </c>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="66"/>
-      <c r="L22" s="68"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
+      <c r="L22" s="72"/>
     </row>
     <row r="23" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B23" s="47">
@@ -1974,10 +1978,10 @@
       <c r="E23" s="47">
         <v>8</v>
       </c>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="66"/>
-      <c r="L23" s="68"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="70"/>
+      <c r="L23" s="72"/>
     </row>
     <row r="24" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B24" s="47">
@@ -1992,10 +1996,10 @@
       <c r="E24" s="47">
         <v>2</v>
       </c>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="66"/>
-      <c r="L24" s="68"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="70"/>
+      <c r="L24" s="72"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="48" t="s">
@@ -2013,17 +2017,17 @@
       <c r="E25" s="16">
         <v>2</v>
       </c>
-      <c r="F25" s="63">
+      <c r="F25" s="67">
         <v>5.75</v>
       </c>
-      <c r="G25" s="64">
-        <v>0</v>
-      </c>
-      <c r="H25" s="62">
+      <c r="G25" s="68">
+        <v>0</v>
+      </c>
+      <c r="H25" s="66">
         <f>F25+G25</f>
         <v>5.75</v>
       </c>
-      <c r="L25" s="61" t="s">
+      <c r="L25" s="65" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2041,10 +2045,10 @@
       <c r="E26" s="16">
         <v>19</v>
       </c>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="62"/>
-      <c r="L26" s="60"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="66"/>
+      <c r="L26" s="64"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="48"/>
@@ -2060,10 +2064,10 @@
       <c r="E27" s="16">
         <v>10</v>
       </c>
-      <c r="F27" s="63"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="62"/>
-      <c r="L27" s="60"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="66"/>
+      <c r="L27" s="64"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="48"/>
@@ -2079,10 +2083,10 @@
       <c r="E28" s="16">
         <v>12</v>
       </c>
-      <c r="F28" s="63"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="62"/>
-      <c r="L28" s="60"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="66"/>
+      <c r="L28" s="64"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="48"/>
@@ -2098,10 +2102,10 @@
       <c r="E29" s="16">
         <v>4</v>
       </c>
-      <c r="F29" s="63"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="62"/>
-      <c r="L29" s="60"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="66"/>
+      <c r="L29" s="64"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="42"/>
@@ -2145,17 +2149,17 @@
       <c r="E31" s="16">
         <v>4</v>
       </c>
-      <c r="F31" s="63">
+      <c r="F31" s="67">
         <v>6.48</v>
       </c>
-      <c r="G31" s="64">
-        <v>0</v>
-      </c>
-      <c r="H31" s="57">
+      <c r="G31" s="68">
+        <v>0</v>
+      </c>
+      <c r="H31" s="61">
         <f>F31+G31</f>
         <v>6.48</v>
       </c>
-      <c r="L31" s="61" t="s">
+      <c r="L31" s="65" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2173,12 +2177,12 @@
       <c r="E32" s="16">
         <v>2</v>
       </c>
-      <c r="F32" s="63"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="57"/>
-      <c r="L32" s="60"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="61"/>
+      <c r="L32" s="64"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="42"/>
       <c r="B33" s="1">
         <v>28</v>
@@ -2206,7 +2210,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="42"/>
       <c r="B34" s="1">
         <v>29</v>
@@ -2234,7 +2238,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="42"/>
       <c r="B35" s="1">
         <v>30</v>
@@ -2262,7 +2266,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="42"/>
       <c r="B36" s="1">
         <v>31</v>
@@ -2290,7 +2294,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="42"/>
       <c r="B37" s="1">
         <v>32</v>
@@ -2318,7 +2322,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="42"/>
       <c r="B38" s="1">
         <v>33</v>
@@ -2346,7 +2350,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="42"/>
       <c r="B39" s="1">
         <v>34</v>
@@ -2374,7 +2378,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="42"/>
       <c r="B40" s="1">
         <v>35</v>
@@ -2388,21 +2392,21 @@
       <c r="E40" s="16">
         <v>2</v>
       </c>
-      <c r="F40" s="59">
+      <c r="F40" s="63">
         <v>0.23</v>
       </c>
-      <c r="G40" s="58">
-        <v>0</v>
-      </c>
-      <c r="H40" s="57">
+      <c r="G40" s="62">
+        <v>0</v>
+      </c>
+      <c r="H40" s="61">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-      <c r="L40" s="60" t="s">
+      <c r="L40" s="64" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="42"/>
       <c r="B41" s="1">
         <v>36</v>
@@ -2416,12 +2420,12 @@
       <c r="E41" s="16">
         <v>4</v>
       </c>
-      <c r="F41" s="59"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="57"/>
-      <c r="L41" s="60"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F41" s="63"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="61"/>
+      <c r="L41" s="64"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="42"/>
       <c r="B42" s="1">
         <v>37</v>
@@ -2435,12 +2439,12 @@
       <c r="E42" s="16">
         <v>4</v>
       </c>
-      <c r="F42" s="59"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="57"/>
-      <c r="L42" s="60"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F42" s="63"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="61"/>
+      <c r="L42" s="64"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="48" t="s">
         <v>236</v>
       </c>
@@ -2470,7 +2474,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="48" t="s">
         <v>237</v>
       </c>
@@ -2500,21 +2504,21 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B45" s="1"/>
       <c r="C45" s="11"/>
       <c r="E45" s="16"/>
       <c r="G45" s="26"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B46" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="19"/>
       <c r="G46" s="29"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B47" s="1">
         <v>40</v>
       </c>
@@ -2538,7 +2542,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A48" s="60"/>
       <c r="B48" s="1">
         <v>41</v>
       </c>
@@ -2561,6 +2566,9 @@
       </c>
       <c r="L48" t="s">
         <v>200</v>
+      </c>
+      <c r="M48" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.45">
@@ -2782,7 +2790,7 @@
       <c r="E62" s="16">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F62" s="59">
+      <c r="F62" s="63">
         <v>25.61</v>
       </c>
       <c r="G62" s="26">
@@ -2806,7 +2814,7 @@
       <c r="E63" s="22">
         <v>0.01</v>
       </c>
-      <c r="F63" s="59"/>
+      <c r="F63" s="63"/>
       <c r="G63" s="26">
         <v>0</v>
       </c>
@@ -2828,7 +2836,7 @@
       <c r="E64" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F64" s="59"/>
+      <c r="F64" s="63"/>
       <c r="G64" s="26">
         <v>0</v>
       </c>
@@ -2850,7 +2858,7 @@
       <c r="E65" s="16">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F65" s="59"/>
+      <c r="F65" s="63"/>
       <c r="G65" s="26">
         <v>0</v>
       </c>
@@ -2872,7 +2880,7 @@
       <c r="E66" s="16">
         <v>1.2E-2</v>
       </c>
-      <c r="F66" s="59"/>
+      <c r="F66" s="63"/>
       <c r="G66" s="26">
         <v>0</v>
       </c>
@@ -2894,7 +2902,7 @@
       <c r="E67" s="16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F67" s="59"/>
+      <c r="F67" s="63"/>
       <c r="G67" s="26">
         <v>0</v>
       </c>
@@ -2916,7 +2924,7 @@
       <c r="E68" s="16">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F68" s="59"/>
+      <c r="F68" s="63"/>
       <c r="G68" s="26">
         <v>0</v>
       </c>
@@ -2938,7 +2946,7 @@
       <c r="E69" s="16">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="F69" s="59"/>
+      <c r="F69" s="63"/>
       <c r="G69" s="26">
         <v>0</v>
       </c>
@@ -2960,7 +2968,7 @@
       <c r="E70" s="16">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F70" s="59"/>
+      <c r="F70" s="63"/>
       <c r="G70" s="26">
         <v>0</v>
       </c>
@@ -2982,7 +2990,7 @@
       <c r="E71" s="16">
         <v>2.4E-2</v>
       </c>
-      <c r="F71" s="59"/>
+      <c r="F71" s="63"/>
       <c r="G71" s="26">
         <v>0</v>
       </c>
@@ -3004,7 +3012,7 @@
       <c r="E72" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F72" s="59"/>
+      <c r="F72" s="63"/>
       <c r="G72" s="26">
         <v>0</v>
       </c>
@@ -3026,7 +3034,7 @@
       <c r="E73" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F73" s="59"/>
+      <c r="F73" s="63"/>
       <c r="G73" s="26">
         <v>0</v>
       </c>
@@ -3048,7 +3056,7 @@
       <c r="E74" s="16">
         <v>1.4E-2</v>
       </c>
-      <c r="F74" s="59"/>
+      <c r="F74" s="63"/>
       <c r="G74" s="26">
         <v>0</v>
       </c>
@@ -3070,7 +3078,7 @@
       <c r="E75" s="16">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F75" s="59"/>
+      <c r="F75" s="63"/>
       <c r="G75" s="26">
         <v>0</v>
       </c>
@@ -3092,7 +3100,7 @@
       <c r="E76" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F76" s="59"/>
+      <c r="F76" s="63"/>
       <c r="G76" s="26">
         <v>0</v>
       </c>
@@ -3114,7 +3122,7 @@
       <c r="E77" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F77" s="59"/>
+      <c r="F77" s="63"/>
       <c r="G77" s="26">
         <v>0</v>
       </c>
@@ -3193,7 +3201,7 @@
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A82" s="69" t="s">
+      <c r="A82" s="57" t="s">
         <v>248</v>
       </c>
       <c r="B82" s="1">
@@ -3221,7 +3229,7 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A83" s="69" t="s">
+      <c r="A83" s="57" t="s">
         <v>249</v>
       </c>
       <c r="B83" s="1">
@@ -3405,7 +3413,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A90" s="71"/>
+      <c r="A90" s="59"/>
       <c r="B90" s="1">
         <v>77</v>
       </c>
@@ -3458,7 +3466,7 @@
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A92" s="69" t="s">
+      <c r="A92" s="57" t="s">
         <v>250</v>
       </c>
       <c r="B92" s="1">
@@ -3656,17 +3664,17 @@
       <c r="E100" s="16">
         <v>2</v>
       </c>
-      <c r="F100" s="59">
+      <c r="F100" s="63">
         <v>0.47</v>
       </c>
-      <c r="G100" s="58">
-        <v>0</v>
-      </c>
-      <c r="H100" s="62">
+      <c r="G100" s="62">
+        <v>0</v>
+      </c>
+      <c r="H100" s="66">
         <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
-      <c r="L100" s="61" t="s">
+      <c r="L100" s="65" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3684,10 +3692,10 @@
       <c r="E101" s="16">
         <v>1</v>
       </c>
-      <c r="F101" s="59"/>
-      <c r="G101" s="58"/>
-      <c r="H101" s="62"/>
-      <c r="L101" s="60"/>
+      <c r="F101" s="63"/>
+      <c r="G101" s="62"/>
+      <c r="H101" s="66"/>
+      <c r="L101" s="64"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A102" s="48"/>
@@ -3703,10 +3711,10 @@
       <c r="E102" s="16">
         <v>4</v>
       </c>
-      <c r="F102" s="59"/>
-      <c r="G102" s="58"/>
-      <c r="H102" s="62"/>
-      <c r="L102" s="60"/>
+      <c r="F102" s="63"/>
+      <c r="G102" s="62"/>
+      <c r="H102" s="66"/>
+      <c r="L102" s="64"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103" s="48"/>
@@ -3722,10 +3730,10 @@
       <c r="E103" s="16">
         <v>1</v>
       </c>
-      <c r="F103" s="59"/>
-      <c r="G103" s="58"/>
-      <c r="H103" s="62"/>
-      <c r="L103" s="60"/>
+      <c r="F103" s="63"/>
+      <c r="G103" s="62"/>
+      <c r="H103" s="66"/>
+      <c r="L103" s="64"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" s="48"/>
@@ -3741,10 +3749,10 @@
       <c r="E104" s="16">
         <v>4</v>
       </c>
-      <c r="F104" s="59"/>
-      <c r="G104" s="58"/>
-      <c r="H104" s="62"/>
-      <c r="L104" s="60"/>
+      <c r="F104" s="63"/>
+      <c r="G104" s="62"/>
+      <c r="H104" s="66"/>
+      <c r="L104" s="64"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" s="48"/>
@@ -3760,10 +3768,10 @@
       <c r="E105" s="16">
         <v>2</v>
       </c>
-      <c r="F105" s="59"/>
-      <c r="G105" s="58"/>
-      <c r="H105" s="62"/>
-      <c r="L105" s="60"/>
+      <c r="F105" s="63"/>
+      <c r="G105" s="62"/>
+      <c r="H105" s="66"/>
+      <c r="L105" s="64"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" s="48"/>
@@ -3779,10 +3787,10 @@
       <c r="E106" s="16">
         <v>1</v>
       </c>
-      <c r="F106" s="59"/>
-      <c r="G106" s="58"/>
-      <c r="H106" s="62"/>
-      <c r="L106" s="60"/>
+      <c r="F106" s="63"/>
+      <c r="G106" s="62"/>
+      <c r="H106" s="66"/>
+      <c r="L106" s="64"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107" s="48" t="s">
@@ -3800,17 +3808,17 @@
       <c r="E107" s="16">
         <v>2</v>
       </c>
-      <c r="F107" s="59">
+      <c r="F107" s="63">
         <v>3.28</v>
       </c>
-      <c r="G107" s="58">
-        <v>0</v>
-      </c>
-      <c r="H107" s="57">
+      <c r="G107" s="62">
+        <v>0</v>
+      </c>
+      <c r="H107" s="61">
         <f t="shared" si="2"/>
         <v>6.56</v>
       </c>
-      <c r="L107" s="61" t="s">
+      <c r="L107" s="65" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3828,10 +3836,10 @@
       <c r="E108" s="16">
         <v>1</v>
       </c>
-      <c r="F108" s="59"/>
-      <c r="G108" s="58"/>
-      <c r="H108" s="57"/>
-      <c r="L108" s="60"/>
+      <c r="F108" s="63"/>
+      <c r="G108" s="62"/>
+      <c r="H108" s="61"/>
+      <c r="L108" s="64"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A109" s="48"/>
@@ -3847,10 +3855,10 @@
       <c r="E109" s="16">
         <v>2</v>
       </c>
-      <c r="F109" s="59"/>
-      <c r="G109" s="58"/>
-      <c r="H109" s="57"/>
-      <c r="L109" s="60"/>
+      <c r="F109" s="63"/>
+      <c r="G109" s="62"/>
+      <c r="H109" s="61"/>
+      <c r="L109" s="64"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A110" s="37" t="s">
@@ -4039,20 +4047,20 @@
       <c r="E116" s="16">
         <v>7</v>
       </c>
-      <c r="F116" s="59">
+      <c r="F116" s="63">
         <v>4.5</v>
       </c>
-      <c r="G116" s="58">
+      <c r="G116" s="62">
         <v>1.89</v>
       </c>
-      <c r="H116" s="57">
+      <c r="H116" s="61">
         <f>F116+G116</f>
         <v>6.39</v>
       </c>
       <c r="I116" s="34"/>
       <c r="J116" s="34"/>
       <c r="K116" s="34"/>
-      <c r="L116" s="60" t="s">
+      <c r="L116" s="64" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4070,13 +4078,13 @@
       <c r="E117" s="16">
         <v>1</v>
       </c>
-      <c r="F117" s="59"/>
-      <c r="G117" s="58"/>
-      <c r="H117" s="57"/>
+      <c r="F117" s="63"/>
+      <c r="G117" s="62"/>
+      <c r="H117" s="61"/>
       <c r="I117" s="34"/>
       <c r="J117" s="34"/>
       <c r="K117" s="34"/>
-      <c r="L117" s="60"/>
+      <c r="L117" s="64"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A118" s="54" t="s">
@@ -4251,7 +4259,7 @@
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A124" s="69" t="s">
+      <c r="A124" s="57" t="s">
         <v>246</v>
       </c>
       <c r="B124" s="1">
@@ -4279,7 +4287,7 @@
       <c r="L124" t="s">
         <v>213</v>
       </c>
-      <c r="M124" s="70" t="s">
+      <c r="M124" s="58" t="s">
         <v>247</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Frame + Fasteners | Found issue with BOM
Having issues with smart fasteners feature
BOM calls for CML50, but I noticed that the scope uses CML100(!)
</commit_message>
<xml_diff>
--- a/BOM/BillOfMaterials.xlsx
+++ b/BOM/BillOfMaterials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reger\Documents\Project\Flex Delft Work\Open Hardware\Schistoscope\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279B9ED5-FF2F-4982-AEE1-EEA6DC6E0175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B86B21-9FAF-477E-B56E-B46AB9E0B039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{E17B2124-711C-4341-A725-6D6BA9A2AA94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="252">
   <si>
     <t>Name</t>
   </si>
@@ -787,6 +787,9 @@
   </si>
   <si>
     <t>Farnelll</t>
+  </si>
+  <si>
+    <t>Scope has CML100(?)</t>
   </si>
 </sst>
 </file>
@@ -986,7 +989,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1076,6 +1079,10 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1112,9 +1119,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1436,8 +1440,8 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1929,17 +1933,17 @@
       <c r="E21" s="47">
         <v>8</v>
       </c>
-      <c r="F21" s="65">
+      <c r="F21" s="69">
         <v>1.84</v>
       </c>
-      <c r="G21" s="65">
-        <v>0</v>
-      </c>
-      <c r="H21" s="66">
+      <c r="G21" s="69">
+        <v>0</v>
+      </c>
+      <c r="H21" s="70">
         <f>F21+G21</f>
         <v>1.84</v>
       </c>
-      <c r="L21" s="67" t="s">
+      <c r="L21" s="71" t="s">
         <v>220</v>
       </c>
     </row>
@@ -1956,10 +1960,10 @@
       <c r="E22" s="47">
         <v>12</v>
       </c>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="66"/>
-      <c r="L22" s="68"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
+      <c r="L22" s="72"/>
     </row>
     <row r="23" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B23" s="47">
@@ -1974,10 +1978,10 @@
       <c r="E23" s="47">
         <v>8</v>
       </c>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="66"/>
-      <c r="L23" s="68"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="70"/>
+      <c r="L23" s="72"/>
     </row>
     <row r="24" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B24" s="47">
@@ -1992,10 +1996,10 @@
       <c r="E24" s="47">
         <v>2</v>
       </c>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="66"/>
-      <c r="L24" s="68"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="70"/>
+      <c r="L24" s="72"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="48" t="s">
@@ -2013,17 +2017,17 @@
       <c r="E25" s="16">
         <v>2</v>
       </c>
-      <c r="F25" s="63">
+      <c r="F25" s="67">
         <v>5.75</v>
       </c>
-      <c r="G25" s="64">
-        <v>0</v>
-      </c>
-      <c r="H25" s="62">
+      <c r="G25" s="68">
+        <v>0</v>
+      </c>
+      <c r="H25" s="66">
         <f>F25+G25</f>
         <v>5.75</v>
       </c>
-      <c r="L25" s="61" t="s">
+      <c r="L25" s="65" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2041,10 +2045,10 @@
       <c r="E26" s="16">
         <v>19</v>
       </c>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="62"/>
-      <c r="L26" s="60"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="66"/>
+      <c r="L26" s="64"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="48"/>
@@ -2060,10 +2064,10 @@
       <c r="E27" s="16">
         <v>10</v>
       </c>
-      <c r="F27" s="63"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="62"/>
-      <c r="L27" s="60"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="66"/>
+      <c r="L27" s="64"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="48"/>
@@ -2079,10 +2083,10 @@
       <c r="E28" s="16">
         <v>12</v>
       </c>
-      <c r="F28" s="63"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="62"/>
-      <c r="L28" s="60"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="66"/>
+      <c r="L28" s="64"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="48"/>
@@ -2098,10 +2102,10 @@
       <c r="E29" s="16">
         <v>4</v>
       </c>
-      <c r="F29" s="63"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="62"/>
-      <c r="L29" s="60"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="66"/>
+      <c r="L29" s="64"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="42"/>
@@ -2145,17 +2149,17 @@
       <c r="E31" s="16">
         <v>4</v>
       </c>
-      <c r="F31" s="63">
+      <c r="F31" s="67">
         <v>6.48</v>
       </c>
-      <c r="G31" s="64">
-        <v>0</v>
-      </c>
-      <c r="H31" s="57">
+      <c r="G31" s="68">
+        <v>0</v>
+      </c>
+      <c r="H31" s="61">
         <f>F31+G31</f>
         <v>6.48</v>
       </c>
-      <c r="L31" s="61" t="s">
+      <c r="L31" s="65" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2173,12 +2177,12 @@
       <c r="E32" s="16">
         <v>2</v>
       </c>
-      <c r="F32" s="63"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="57"/>
-      <c r="L32" s="60"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="61"/>
+      <c r="L32" s="64"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="42"/>
       <c r="B33" s="1">
         <v>28</v>
@@ -2206,7 +2210,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="42"/>
       <c r="B34" s="1">
         <v>29</v>
@@ -2234,7 +2238,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="42"/>
       <c r="B35" s="1">
         <v>30</v>
@@ -2262,7 +2266,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="42"/>
       <c r="B36" s="1">
         <v>31</v>
@@ -2290,7 +2294,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="42"/>
       <c r="B37" s="1">
         <v>32</v>
@@ -2318,7 +2322,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="42"/>
       <c r="B38" s="1">
         <v>33</v>
@@ -2346,7 +2350,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="42"/>
       <c r="B39" s="1">
         <v>34</v>
@@ -2374,7 +2378,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="42"/>
       <c r="B40" s="1">
         <v>35</v>
@@ -2388,21 +2392,21 @@
       <c r="E40" s="16">
         <v>2</v>
       </c>
-      <c r="F40" s="59">
+      <c r="F40" s="63">
         <v>0.23</v>
       </c>
-      <c r="G40" s="58">
-        <v>0</v>
-      </c>
-      <c r="H40" s="57">
+      <c r="G40" s="62">
+        <v>0</v>
+      </c>
+      <c r="H40" s="61">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-      <c r="L40" s="60" t="s">
+      <c r="L40" s="64" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="42"/>
       <c r="B41" s="1">
         <v>36</v>
@@ -2416,12 +2420,12 @@
       <c r="E41" s="16">
         <v>4</v>
       </c>
-      <c r="F41" s="59"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="57"/>
-      <c r="L41" s="60"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F41" s="63"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="61"/>
+      <c r="L41" s="64"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="42"/>
       <c r="B42" s="1">
         <v>37</v>
@@ -2435,12 +2439,12 @@
       <c r="E42" s="16">
         <v>4</v>
       </c>
-      <c r="F42" s="59"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="57"/>
-      <c r="L42" s="60"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F42" s="63"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="61"/>
+      <c r="L42" s="64"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="48" t="s">
         <v>236</v>
       </c>
@@ -2470,7 +2474,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="48" t="s">
         <v>237</v>
       </c>
@@ -2500,21 +2504,21 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B45" s="1"/>
       <c r="C45" s="11"/>
       <c r="E45" s="16"/>
       <c r="G45" s="26"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B46" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="19"/>
       <c r="G46" s="29"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B47" s="1">
         <v>40</v>
       </c>
@@ -2538,7 +2542,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A48" s="60"/>
       <c r="B48" s="1">
         <v>41</v>
       </c>
@@ -2561,6 +2566,9 @@
       </c>
       <c r="L48" t="s">
         <v>200</v>
+      </c>
+      <c r="M48" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.45">
@@ -2782,7 +2790,7 @@
       <c r="E62" s="16">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F62" s="59">
+      <c r="F62" s="63">
         <v>25.61</v>
       </c>
       <c r="G62" s="26">
@@ -2806,7 +2814,7 @@
       <c r="E63" s="22">
         <v>0.01</v>
       </c>
-      <c r="F63" s="59"/>
+      <c r="F63" s="63"/>
       <c r="G63" s="26">
         <v>0</v>
       </c>
@@ -2828,7 +2836,7 @@
       <c r="E64" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F64" s="59"/>
+      <c r="F64" s="63"/>
       <c r="G64" s="26">
         <v>0</v>
       </c>
@@ -2850,7 +2858,7 @@
       <c r="E65" s="16">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F65" s="59"/>
+      <c r="F65" s="63"/>
       <c r="G65" s="26">
         <v>0</v>
       </c>
@@ -2872,7 +2880,7 @@
       <c r="E66" s="16">
         <v>1.2E-2</v>
       </c>
-      <c r="F66" s="59"/>
+      <c r="F66" s="63"/>
       <c r="G66" s="26">
         <v>0</v>
       </c>
@@ -2894,7 +2902,7 @@
       <c r="E67" s="16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F67" s="59"/>
+      <c r="F67" s="63"/>
       <c r="G67" s="26">
         <v>0</v>
       </c>
@@ -2916,7 +2924,7 @@
       <c r="E68" s="16">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F68" s="59"/>
+      <c r="F68" s="63"/>
       <c r="G68" s="26">
         <v>0</v>
       </c>
@@ -2938,7 +2946,7 @@
       <c r="E69" s="16">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="F69" s="59"/>
+      <c r="F69" s="63"/>
       <c r="G69" s="26">
         <v>0</v>
       </c>
@@ -2960,7 +2968,7 @@
       <c r="E70" s="16">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F70" s="59"/>
+      <c r="F70" s="63"/>
       <c r="G70" s="26">
         <v>0</v>
       </c>
@@ -2982,7 +2990,7 @@
       <c r="E71" s="16">
         <v>2.4E-2</v>
       </c>
-      <c r="F71" s="59"/>
+      <c r="F71" s="63"/>
       <c r="G71" s="26">
         <v>0</v>
       </c>
@@ -3004,7 +3012,7 @@
       <c r="E72" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F72" s="59"/>
+      <c r="F72" s="63"/>
       <c r="G72" s="26">
         <v>0</v>
       </c>
@@ -3026,7 +3034,7 @@
       <c r="E73" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F73" s="59"/>
+      <c r="F73" s="63"/>
       <c r="G73" s="26">
         <v>0</v>
       </c>
@@ -3048,7 +3056,7 @@
       <c r="E74" s="16">
         <v>1.4E-2</v>
       </c>
-      <c r="F74" s="59"/>
+      <c r="F74" s="63"/>
       <c r="G74" s="26">
         <v>0</v>
       </c>
@@ -3070,7 +3078,7 @@
       <c r="E75" s="16">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F75" s="59"/>
+      <c r="F75" s="63"/>
       <c r="G75" s="26">
         <v>0</v>
       </c>
@@ -3092,7 +3100,7 @@
       <c r="E76" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F76" s="59"/>
+      <c r="F76" s="63"/>
       <c r="G76" s="26">
         <v>0</v>
       </c>
@@ -3114,7 +3122,7 @@
       <c r="E77" s="16">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F77" s="59"/>
+      <c r="F77" s="63"/>
       <c r="G77" s="26">
         <v>0</v>
       </c>
@@ -3193,7 +3201,7 @@
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A82" s="69" t="s">
+      <c r="A82" s="57" t="s">
         <v>248</v>
       </c>
       <c r="B82" s="1">
@@ -3221,7 +3229,7 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A83" s="69" t="s">
+      <c r="A83" s="57" t="s">
         <v>249</v>
       </c>
       <c r="B83" s="1">
@@ -3405,7 +3413,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A90" s="71"/>
+      <c r="A90" s="59"/>
       <c r="B90" s="1">
         <v>77</v>
       </c>
@@ -3458,7 +3466,7 @@
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A92" s="69" t="s">
+      <c r="A92" s="57" t="s">
         <v>250</v>
       </c>
       <c r="B92" s="1">
@@ -3656,17 +3664,17 @@
       <c r="E100" s="16">
         <v>2</v>
       </c>
-      <c r="F100" s="59">
+      <c r="F100" s="63">
         <v>0.47</v>
       </c>
-      <c r="G100" s="58">
-        <v>0</v>
-      </c>
-      <c r="H100" s="62">
+      <c r="G100" s="62">
+        <v>0</v>
+      </c>
+      <c r="H100" s="66">
         <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
-      <c r="L100" s="61" t="s">
+      <c r="L100" s="65" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3684,10 +3692,10 @@
       <c r="E101" s="16">
         <v>1</v>
       </c>
-      <c r="F101" s="59"/>
-      <c r="G101" s="58"/>
-      <c r="H101" s="62"/>
-      <c r="L101" s="60"/>
+      <c r="F101" s="63"/>
+      <c r="G101" s="62"/>
+      <c r="H101" s="66"/>
+      <c r="L101" s="64"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A102" s="48"/>
@@ -3703,10 +3711,10 @@
       <c r="E102" s="16">
         <v>4</v>
       </c>
-      <c r="F102" s="59"/>
-      <c r="G102" s="58"/>
-      <c r="H102" s="62"/>
-      <c r="L102" s="60"/>
+      <c r="F102" s="63"/>
+      <c r="G102" s="62"/>
+      <c r="H102" s="66"/>
+      <c r="L102" s="64"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103" s="48"/>
@@ -3722,10 +3730,10 @@
       <c r="E103" s="16">
         <v>1</v>
       </c>
-      <c r="F103" s="59"/>
-      <c r="G103" s="58"/>
-      <c r="H103" s="62"/>
-      <c r="L103" s="60"/>
+      <c r="F103" s="63"/>
+      <c r="G103" s="62"/>
+      <c r="H103" s="66"/>
+      <c r="L103" s="64"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" s="48"/>
@@ -3741,10 +3749,10 @@
       <c r="E104" s="16">
         <v>4</v>
       </c>
-      <c r="F104" s="59"/>
-      <c r="G104" s="58"/>
-      <c r="H104" s="62"/>
-      <c r="L104" s="60"/>
+      <c r="F104" s="63"/>
+      <c r="G104" s="62"/>
+      <c r="H104" s="66"/>
+      <c r="L104" s="64"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" s="48"/>
@@ -3760,10 +3768,10 @@
       <c r="E105" s="16">
         <v>2</v>
       </c>
-      <c r="F105" s="59"/>
-      <c r="G105" s="58"/>
-      <c r="H105" s="62"/>
-      <c r="L105" s="60"/>
+      <c r="F105" s="63"/>
+      <c r="G105" s="62"/>
+      <c r="H105" s="66"/>
+      <c r="L105" s="64"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" s="48"/>
@@ -3779,10 +3787,10 @@
       <c r="E106" s="16">
         <v>1</v>
       </c>
-      <c r="F106" s="59"/>
-      <c r="G106" s="58"/>
-      <c r="H106" s="62"/>
-      <c r="L106" s="60"/>
+      <c r="F106" s="63"/>
+      <c r="G106" s="62"/>
+      <c r="H106" s="66"/>
+      <c r="L106" s="64"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107" s="48" t="s">
@@ -3800,17 +3808,17 @@
       <c r="E107" s="16">
         <v>2</v>
       </c>
-      <c r="F107" s="59">
+      <c r="F107" s="63">
         <v>3.28</v>
       </c>
-      <c r="G107" s="58">
-        <v>0</v>
-      </c>
-      <c r="H107" s="57">
+      <c r="G107" s="62">
+        <v>0</v>
+      </c>
+      <c r="H107" s="61">
         <f t="shared" si="2"/>
         <v>6.56</v>
       </c>
-      <c r="L107" s="61" t="s">
+      <c r="L107" s="65" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3828,10 +3836,10 @@
       <c r="E108" s="16">
         <v>1</v>
       </c>
-      <c r="F108" s="59"/>
-      <c r="G108" s="58"/>
-      <c r="H108" s="57"/>
-      <c r="L108" s="60"/>
+      <c r="F108" s="63"/>
+      <c r="G108" s="62"/>
+      <c r="H108" s="61"/>
+      <c r="L108" s="64"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A109" s="48"/>
@@ -3847,10 +3855,10 @@
       <c r="E109" s="16">
         <v>2</v>
       </c>
-      <c r="F109" s="59"/>
-      <c r="G109" s="58"/>
-      <c r="H109" s="57"/>
-      <c r="L109" s="60"/>
+      <c r="F109" s="63"/>
+      <c r="G109" s="62"/>
+      <c r="H109" s="61"/>
+      <c r="L109" s="64"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A110" s="37" t="s">
@@ -4039,20 +4047,20 @@
       <c r="E116" s="16">
         <v>7</v>
       </c>
-      <c r="F116" s="59">
+      <c r="F116" s="63">
         <v>4.5</v>
       </c>
-      <c r="G116" s="58">
+      <c r="G116" s="62">
         <v>1.89</v>
       </c>
-      <c r="H116" s="57">
+      <c r="H116" s="61">
         <f>F116+G116</f>
         <v>6.39</v>
       </c>
       <c r="I116" s="34"/>
       <c r="J116" s="34"/>
       <c r="K116" s="34"/>
-      <c r="L116" s="60" t="s">
+      <c r="L116" s="64" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4070,13 +4078,13 @@
       <c r="E117" s="16">
         <v>1</v>
       </c>
-      <c r="F117" s="59"/>
-      <c r="G117" s="58"/>
-      <c r="H117" s="57"/>
+      <c r="F117" s="63"/>
+      <c r="G117" s="62"/>
+      <c r="H117" s="61"/>
       <c r="I117" s="34"/>
       <c r="J117" s="34"/>
       <c r="K117" s="34"/>
-      <c r="L117" s="60"/>
+      <c r="L117" s="64"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A118" s="54" t="s">
@@ -4251,7 +4259,7 @@
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A124" s="69" t="s">
+      <c r="A124" s="57" t="s">
         <v>246</v>
       </c>
       <c r="B124" s="1">
@@ -4279,7 +4287,7 @@
       <c r="L124" t="s">
         <v>213</v>
       </c>
-      <c r="M124" s="70" t="s">
+      <c r="M124" s="58" t="s">
         <v>247</v>
       </c>
     </row>

</xml_diff>